<commit_message>
don't need biomark marker tags as "test tags" in metadata anymore
</commit_message>
<xml_diff>
--- a/data/WGFP Metadata.xlsx
+++ b/data/WGFP Metadata.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072"/>
   </bookViews>
   <sheets>
     <sheet name="AntennaMetadata" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="52">
   <si>
     <t>Variable</t>
   </si>
@@ -151,9 +151,6 @@
     <t>type</t>
   </si>
   <si>
-    <t>Biomark Marker Tag</t>
-  </si>
-  <si>
     <t>?</t>
   </si>
   <si>
@@ -176,6 +173,15 @@
   </si>
   <si>
     <t>55 detections in 2023: 6/6, 6/23. 7/25 at RB, CF and HP</t>
+  </si>
+  <si>
+    <t>4 detections on 2020-10-08 at CF</t>
+  </si>
+  <si>
+    <t>notes</t>
+  </si>
+  <si>
+    <t>no detections</t>
   </si>
 </sst>
 </file>
@@ -497,13 +503,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="42.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -796,15 +802,17 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="26.6640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="28.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="76.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
@@ -814,13 +822,16 @@
       <c r="B1" t="s">
         <v>40</v>
       </c>
+      <c r="C1" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>900230000102751</v>
       </c>
       <c r="B2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -828,119 +839,99 @@
         <v>900226001581072</v>
       </c>
       <c r="B3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>900230000004000</v>
       </c>
+      <c r="C4" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
-        <v>999000000007586</v>
-      </c>
-      <c r="B5" t="s">
-        <v>41</v>
+        <v>900230000087405</v>
+      </c>
+      <c r="C5" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
-        <v>999000000007585</v>
+        <v>900230000087408</v>
       </c>
       <c r="B6" t="s">
         <v>41</v>
       </c>
+      <c r="C6" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
-        <v>999000000007601</v>
+        <v>900226001546996</v>
       </c>
       <c r="B7" t="s">
         <v>41</v>
       </c>
+      <c r="C7" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
-        <v>999000000007602</v>
-      </c>
-      <c r="B8" t="s">
-        <v>41</v>
+        <v>900230000088083</v>
+      </c>
+      <c r="C8" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
-        <v>900230000087405</v>
+        <v>900230000087402</v>
+      </c>
+      <c r="B9" t="s">
+        <v>41</v>
+      </c>
+      <c r="C9" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
-        <v>900230000087408</v>
+        <v>900230000087403</v>
       </c>
       <c r="B10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C10" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
-        <v>900226001546996</v>
-      </c>
-      <c r="B11" t="s">
-        <v>42</v>
+        <v>900230000088082</v>
       </c>
       <c r="C11" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
-        <v>900230000088083</v>
+        <v>900230000228791</v>
       </c>
       <c r="C12" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
-        <v>900230000087402</v>
-      </c>
-      <c r="B13" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="2">
-        <v>900230000087403</v>
-      </c>
-      <c r="B14" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" s="2">
-        <v>900230000088082</v>
-      </c>
-      <c r="C15" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" s="2">
-        <v>900230000228791</v>
-      </c>
-      <c r="C16" t="s">
+        <v>900230000087401</v>
+      </c>
+      <c r="C13" t="s">
         <v>48</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="2">
-        <v>900230000087401</v>
-      </c>
-      <c r="C17" t="s">
-        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
slowly incporating metadata: allcombinedEventsFunction
</commit_message>
<xml_diff>
--- a/data/WGFP Metadata.xlsx
+++ b/data/WGFP Metadata.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="58">
   <si>
     <t>Variable</t>
   </si>
@@ -34,9 +34,6 @@
     <t>AntennaSite</t>
   </si>
   <si>
-    <t>Abbreviation</t>
-  </si>
-  <si>
     <t>UTM_X</t>
   </si>
   <si>
@@ -61,9 +58,6 @@
     <t>Fraser River Canyon</t>
   </si>
   <si>
-    <t>Below Windy Gap Dam</t>
-  </si>
-  <si>
     <t>Kaibab Park</t>
   </si>
   <si>
@@ -182,6 +176,30 @@
   </si>
   <si>
     <t>no detections</t>
+  </si>
+  <si>
+    <t>SiteName</t>
+  </si>
+  <si>
+    <t>Red Barn</t>
+  </si>
+  <si>
+    <t>Hitching Post</t>
+  </si>
+  <si>
+    <t>Confluence</t>
+  </si>
+  <si>
+    <t>Connectivity Channel Downstream</t>
+  </si>
+  <si>
+    <t>Connectivity Channel Side Channel</t>
+  </si>
+  <si>
+    <t>Connectivity Channel Upstream</t>
+  </si>
+  <si>
+    <t>SiteCode</t>
   </si>
 </sst>
 </file>
@@ -501,253 +519,305 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="42.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="42.33203125" customWidth="1"/>
+    <col min="3" max="3" width="11.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>1</v>
       </c>
       <c r="B1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2">
+        <v>416026</v>
+      </c>
+      <c r="E2">
+        <v>4440196</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3">
+        <v>420728</v>
+      </c>
+      <c r="E3">
+        <v>4437221</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>11</v>
       </c>
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2">
-        <v>416026</v>
-      </c>
-      <c r="D2">
-        <v>4440196</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
         <v>7</v>
       </c>
-      <c r="C3">
-        <v>420728</v>
-      </c>
-      <c r="D3">
-        <v>4437221</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4">
+      <c r="D4">
         <v>419210</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <v>4439961</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B5" t="s">
         <v>9</v>
       </c>
-      <c r="C5">
+      <c r="C5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5">
         <v>424543</v>
       </c>
-      <c r="D5">
+      <c r="E5">
         <v>4435559</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6">
+        <v>412489</v>
+      </c>
+      <c r="E6">
+        <v>4439413</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" t="s">
+        <v>51</v>
+      </c>
+      <c r="C7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7">
+        <v>412489</v>
+      </c>
+      <c r="E7" s="1">
+        <v>4439413</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" t="s">
+        <v>52</v>
+      </c>
+      <c r="C8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8">
+        <v>414375</v>
+      </c>
+      <c r="E8">
+        <v>4440241</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>17</v>
       </c>
-      <c r="B6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6">
-        <v>412489</v>
-      </c>
-      <c r="D6">
-        <v>4439413</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+      <c r="B9" t="s">
+        <v>52</v>
+      </c>
+      <c r="C9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9">
+        <v>414375</v>
+      </c>
+      <c r="E9">
+        <v>4440241</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
         <v>18</v>
       </c>
-      <c r="B7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7">
-        <v>412489</v>
-      </c>
-      <c r="D7" s="1">
-        <v>4439413</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8" t="s">
+      <c r="B10" t="s">
+        <v>53</v>
+      </c>
+      <c r="C10" t="s">
         <v>22</v>
       </c>
-      <c r="C8">
-        <v>414375</v>
-      </c>
-      <c r="D8">
-        <v>4440241</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+      <c r="D10">
+        <v>416965</v>
+      </c>
+      <c r="E10">
+        <v>4439369</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
         <v>19</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B11" t="s">
+        <v>53</v>
+      </c>
+      <c r="C11" t="s">
         <v>23</v>
       </c>
-      <c r="C9">
-        <v>414375</v>
-      </c>
-      <c r="D9">
-        <v>4440241</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>20</v>
-      </c>
-      <c r="B10" t="s">
+      <c r="D11">
+        <v>416965</v>
+      </c>
+      <c r="E11">
+        <v>4439369</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
         <v>24</v>
       </c>
-      <c r="C10">
-        <v>416965</v>
-      </c>
-      <c r="D10">
-        <v>4439369</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>21</v>
-      </c>
-      <c r="B11" t="s">
+      <c r="B12" t="s">
+        <v>54</v>
+      </c>
+      <c r="C12" t="s">
         <v>25</v>
       </c>
-      <c r="C11">
-        <v>416965</v>
-      </c>
-      <c r="D11">
-        <v>4439369</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+      <c r="D12">
+        <v>415802</v>
+      </c>
+      <c r="E12">
+        <v>4439907</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" t="s">
+        <v>54</v>
+      </c>
+      <c r="C13" t="s">
         <v>26</v>
       </c>
-      <c r="B12" t="s">
+      <c r="D13">
+        <v>415802</v>
+      </c>
+      <c r="E13">
+        <v>4439907</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14" t="s">
+        <v>55</v>
+      </c>
+      <c r="C14" t="s">
         <v>27</v>
       </c>
-      <c r="C12">
-        <v>415802</v>
-      </c>
-      <c r="D12">
-        <v>4439907</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>26</v>
-      </c>
-      <c r="B13" t="s">
+      <c r="D14">
+        <v>415787</v>
+      </c>
+      <c r="E14">
+        <v>4439908</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>32</v>
+      </c>
+      <c r="B15" t="s">
+        <v>55</v>
+      </c>
+      <c r="C15" t="s">
         <v>28</v>
       </c>
-      <c r="C13">
-        <v>415802</v>
-      </c>
-      <c r="D13">
-        <v>4439907</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+      <c r="D15">
+        <v>415787</v>
+      </c>
+      <c r="E15">
+        <v>4439908</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
         <v>33</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B16" t="s">
+        <v>56</v>
+      </c>
+      <c r="C16" t="s">
         <v>29</v>
       </c>
-      <c r="C14">
-        <v>415787</v>
-      </c>
-      <c r="D14">
-        <v>4439908</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
+      <c r="D16">
+        <v>416723</v>
+      </c>
+      <c r="E16">
+        <v>4439443</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
         <v>34</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B17" t="s">
+        <v>56</v>
+      </c>
+      <c r="C17" t="s">
         <v>30</v>
       </c>
-      <c r="C15">
-        <v>415787</v>
-      </c>
-      <c r="D15">
-        <v>4439908</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>35</v>
-      </c>
-      <c r="B16" t="s">
-        <v>31</v>
-      </c>
-      <c r="C16">
+      <c r="D17">
         <v>416723</v>
       </c>
-      <c r="D16">
-        <v>4439443</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>36</v>
-      </c>
-      <c r="B17" t="s">
-        <v>32</v>
-      </c>
-      <c r="C17">
-        <v>416723</v>
-      </c>
-      <c r="D17">
+      <c r="E17">
         <v>4439443</v>
       </c>
     </row>
@@ -776,12 +846,12 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B2">
         <v>10120</v>
@@ -789,7 +859,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B3">
         <v>8330</v>
@@ -817,13 +887,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -831,7 +901,7 @@
         <v>900230000102751</v>
       </c>
       <c r="B2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -839,7 +909,7 @@
         <v>900226001581072</v>
       </c>
       <c r="B3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -847,7 +917,7 @@
         <v>900230000004000</v>
       </c>
       <c r="C4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -855,7 +925,7 @@
         <v>900230000087405</v>
       </c>
       <c r="C5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -863,10 +933,10 @@
         <v>900230000087408</v>
       </c>
       <c r="B6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C6" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -874,10 +944,10 @@
         <v>900226001546996</v>
       </c>
       <c r="B7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7" t="s">
         <v>41</v>
-      </c>
-      <c r="C7" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
@@ -885,7 +955,7 @@
         <v>900230000088083</v>
       </c>
       <c r="C8" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -893,10 +963,10 @@
         <v>900230000087402</v>
       </c>
       <c r="B9" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C9" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
@@ -904,10 +974,10 @@
         <v>900230000087403</v>
       </c>
       <c r="B10" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C10" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
@@ -915,7 +985,7 @@
         <v>900230000088082</v>
       </c>
       <c r="C11" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
@@ -923,7 +993,7 @@
         <v>900230000228791</v>
       </c>
       <c r="C12" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
@@ -931,7 +1001,7 @@
         <v>900230000087401</v>
       </c>
       <c r="C13" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
preparefoRmovementsStates and summaries metadata incoporiation
work in progress
</commit_message>
<xml_diff>
--- a/data/WGFP Metadata.xlsx
+++ b/data/WGFP Metadata.xlsx
@@ -13,8 +13,9 @@
   </bookViews>
   <sheets>
     <sheet name="AntennaMetadata" sheetId="1" r:id="rId1"/>
-    <sheet name="ImportantStationingVariables" sheetId="2" r:id="rId2"/>
-    <sheet name="TestTags" sheetId="3" r:id="rId3"/>
+    <sheet name="Notes" sheetId="4" r:id="rId2"/>
+    <sheet name="ImportantStationingVariables" sheetId="2" r:id="rId3"/>
+    <sheet name="TestTags" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="70">
   <si>
     <t>Variable</t>
   </si>
@@ -181,25 +182,61 @@
     <t>SiteName</t>
   </si>
   <si>
-    <t>Red Barn</t>
-  </si>
-  <si>
-    <t>Hitching Post</t>
-  </si>
-  <si>
-    <t>Confluence</t>
-  </si>
-  <si>
-    <t>Connectivity Channel Downstream</t>
-  </si>
-  <si>
-    <t>Connectivity Channel Side Channel</t>
-  </si>
-  <si>
-    <t>Connectivity Channel Upstream</t>
-  </si>
-  <si>
     <t>SiteCode</t>
+  </si>
+  <si>
+    <t>River</t>
+  </si>
+  <si>
+    <t>Colorado River</t>
+  </si>
+  <si>
+    <t>Fraser River</t>
+  </si>
+  <si>
+    <t>Connectivity Channel</t>
+  </si>
+  <si>
+    <t>Assumes that for AntennaMetadata, SiteName and River will not be changing. If they do change, you'll have to go into the runscript and ac couple functions including "PrepareforMovementsStatesand Summaries" to change how those variabels are located</t>
+  </si>
+  <si>
+    <t>Windy Gap Dam Biomark Antenna</t>
+  </si>
+  <si>
+    <t>Kaibab Park Biomark Antenna</t>
+  </si>
+  <si>
+    <t>River Run Biomark Antenna</t>
+  </si>
+  <si>
+    <t>Fraser River Canyon Biomark Antenna</t>
+  </si>
+  <si>
+    <t>Red Barn Stationary Antenna</t>
+  </si>
+  <si>
+    <t>Hitching Post Stationary Antenna</t>
+  </si>
+  <si>
+    <t>Confluence Stationary Antenna</t>
+  </si>
+  <si>
+    <t>Connectivity Channel Downstream Stationary Antenna</t>
+  </si>
+  <si>
+    <t>Connectivity Channel Side Channel Stationary Antenna</t>
+  </si>
+  <si>
+    <t>Connectivity Channel Upstream Stationary Antenna</t>
+  </si>
+  <si>
+    <t>M1</t>
+  </si>
+  <si>
+    <t>M2</t>
+  </si>
+  <si>
+    <t>Mobile Run</t>
   </si>
 </sst>
 </file>
@@ -519,10 +556,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -532,7 +569,7 @@
     <col min="3" max="3" width="11.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -540,7 +577,7 @@
         <v>50</v>
       </c>
       <c r="C1" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
@@ -548,13 +585,16 @@
       <c r="E1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>36</v>
       </c>
       <c r="B2" t="s">
-        <v>36</v>
+        <v>57</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>
@@ -565,13 +605,16 @@
       <c r="E2">
         <v>4440196</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>58</v>
       </c>
       <c r="C3" t="s">
         <v>6</v>
@@ -582,13 +625,16 @@
       <c r="E3">
         <v>4437221</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>59</v>
       </c>
       <c r="C4" t="s">
         <v>7</v>
@@ -599,13 +645,16 @@
       <c r="E4">
         <v>4439961</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>60</v>
       </c>
       <c r="C5" t="s">
         <v>8</v>
@@ -616,13 +665,16 @@
       <c r="E5">
         <v>4435559</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>15</v>
       </c>
       <c r="B6" t="s">
-        <v>51</v>
+        <v>61</v>
       </c>
       <c r="C6" t="s">
         <v>12</v>
@@ -633,13 +685,16 @@
       <c r="E6">
         <v>4439413</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F6" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>16</v>
       </c>
       <c r="B7" t="s">
-        <v>51</v>
+        <v>61</v>
       </c>
       <c r="C7" t="s">
         <v>13</v>
@@ -650,13 +705,16 @@
       <c r="E7" s="1">
         <v>4439413</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F7" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="C8" t="s">
         <v>20</v>
@@ -667,13 +725,16 @@
       <c r="E8">
         <v>4440241</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F8" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>17</v>
       </c>
       <c r="B9" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="C9" t="s">
         <v>21</v>
@@ -684,13 +745,16 @@
       <c r="E9">
         <v>4440241</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F9" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>18</v>
       </c>
       <c r="B10" t="s">
-        <v>53</v>
+        <v>63</v>
       </c>
       <c r="C10" t="s">
         <v>22</v>
@@ -701,13 +765,16 @@
       <c r="E10">
         <v>4439369</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F10" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>19</v>
       </c>
       <c r="B11" t="s">
-        <v>53</v>
+        <v>63</v>
       </c>
       <c r="C11" t="s">
         <v>23</v>
@@ -718,13 +785,16 @@
       <c r="E11">
         <v>4439369</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F11" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>24</v>
       </c>
       <c r="B12" t="s">
-        <v>54</v>
+        <v>64</v>
       </c>
       <c r="C12" t="s">
         <v>25</v>
@@ -735,13 +805,16 @@
       <c r="E12">
         <v>4439907</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F12" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>24</v>
       </c>
       <c r="B13" t="s">
-        <v>54</v>
+        <v>64</v>
       </c>
       <c r="C13" t="s">
         <v>26</v>
@@ -752,13 +825,16 @@
       <c r="E13">
         <v>4439907</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F13" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>31</v>
       </c>
       <c r="B14" t="s">
-        <v>55</v>
+        <v>65</v>
       </c>
       <c r="C14" t="s">
         <v>27</v>
@@ -769,13 +845,16 @@
       <c r="E14">
         <v>4439908</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F14" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>32</v>
       </c>
       <c r="B15" t="s">
-        <v>55</v>
+        <v>65</v>
       </c>
       <c r="C15" t="s">
         <v>28</v>
@@ -786,13 +865,16 @@
       <c r="E15">
         <v>4439908</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F15" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>33</v>
       </c>
       <c r="B16" t="s">
-        <v>56</v>
+        <v>66</v>
       </c>
       <c r="C16" t="s">
         <v>29</v>
@@ -803,13 +885,16 @@
       <c r="E16">
         <v>4439443</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F16" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>34</v>
       </c>
       <c r="B17" t="s">
-        <v>56</v>
+        <v>66</v>
       </c>
       <c r="C17" t="s">
         <v>30</v>
@@ -819,6 +904,25 @@
       </c>
       <c r="E17">
         <v>4439443</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B18" t="s">
+        <v>69</v>
+      </c>
+      <c r="C18" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B19" t="s">
+        <v>69</v>
+      </c>
+      <c r="C19" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -829,10 +933,30 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -870,7 +994,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C13"/>
   <sheetViews>

</xml_diff>

<commit_message>
new biomark antenna name working for new data
</commit_message>
<xml_diff>
--- a/data/WGFP Metadata.xlsx
+++ b/data/WGFP Metadata.xlsx
@@ -9,13 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="AntennaMetadata" sheetId="1" r:id="rId1"/>
-    <sheet name="Notes" sheetId="4" r:id="rId2"/>
-    <sheet name="ImportantStationingVariables" sheetId="2" r:id="rId3"/>
-    <sheet name="TestTags" sheetId="3" r:id="rId4"/>
+    <sheet name="ImportantStationingVariables" sheetId="2" r:id="rId2"/>
+    <sheet name="TestTags" sheetId="3" r:id="rId3"/>
+    <sheet name="Notes" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -44,9 +44,6 @@
     <t>StationingLocation</t>
   </si>
   <si>
-    <t>B3</t>
-  </si>
-  <si>
     <t>B4</t>
   </si>
   <si>
@@ -240,6 +237,9 @@
   </si>
   <si>
     <t xml:space="preserve">Connectivity Channel Downstream (Upstream) </t>
+  </si>
+  <si>
+    <t>WG3</t>
   </si>
 </sst>
 </file>
@@ -561,8 +561,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -577,10 +577,10 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C1" t="s">
         <v>50</v>
-      </c>
-      <c r="C1" t="s">
-        <v>51</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
@@ -589,18 +589,18 @@
         <v>3</v>
       </c>
       <c r="F1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>70</v>
       </c>
       <c r="D2">
         <v>416026</v>
@@ -609,18 +609,18 @@
         <v>4440196</v>
       </c>
       <c r="F2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D3">
         <v>420728</v>
@@ -629,18 +629,18 @@
         <v>4437221</v>
       </c>
       <c r="F3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D4">
         <v>419210</v>
@@ -649,18 +649,18 @@
         <v>4439961</v>
       </c>
       <c r="F4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D5">
         <v>424543</v>
@@ -669,18 +669,18 @@
         <v>4435559</v>
       </c>
       <c r="F5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D6">
         <v>412489</v>
@@ -689,18 +689,18 @@
         <v>4439413</v>
       </c>
       <c r="F6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D7">
         <v>412489</v>
@@ -709,18 +709,18 @@
         <v>4439413</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D8">
         <v>414375</v>
@@ -729,18 +729,18 @@
         <v>4440241</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D9">
         <v>414375</v>
@@ -749,18 +749,18 @@
         <v>4440241</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D10">
         <v>416965</v>
@@ -769,18 +769,18 @@
         <v>4439369</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D11">
         <v>416965</v>
@@ -789,18 +789,18 @@
         <v>4439369</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" t="s">
+        <v>63</v>
+      </c>
+      <c r="C12" t="s">
         <v>24</v>
-      </c>
-      <c r="B12" t="s">
-        <v>64</v>
-      </c>
-      <c r="C12" t="s">
-        <v>25</v>
       </c>
       <c r="D12">
         <v>415802</v>
@@ -809,18 +809,18 @@
         <v>4439907</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B13" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D13">
         <v>415802</v>
@@ -829,18 +829,18 @@
         <v>4439907</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B14" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D14">
         <v>415787</v>
@@ -849,18 +849,18 @@
         <v>4439908</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B15" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D15">
         <v>415787</v>
@@ -869,18 +869,18 @@
         <v>4439908</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B16" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D16">
         <v>416723</v>
@@ -889,18 +889,18 @@
         <v>4439443</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B17" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C17" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D17">
         <v>416723</v>
@@ -909,23 +909,23 @@
         <v>4439443</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C18" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C19" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -935,26 +935,6 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
@@ -978,7 +958,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B2">
         <v>10120</v>
@@ -986,7 +966,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B3">
         <v>8330</v>
@@ -997,12 +977,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1014,13 +994,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" t="s">
         <v>37</v>
       </c>
-      <c r="B1" t="s">
-        <v>38</v>
-      </c>
       <c r="C1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -1028,7 +1008,7 @@
         <v>900230000102751</v>
       </c>
       <c r="B2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -1036,7 +1016,7 @@
         <v>900226001581072</v>
       </c>
       <c r="B3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -1044,7 +1024,7 @@
         <v>900230000004000</v>
       </c>
       <c r="C4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -1052,7 +1032,7 @@
         <v>900230000087405</v>
       </c>
       <c r="C5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -1060,10 +1040,10 @@
         <v>900230000087408</v>
       </c>
       <c r="B6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C6" t="s">
         <v>39</v>
-      </c>
-      <c r="C6" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -1071,10 +1051,10 @@
         <v>900226001546996</v>
       </c>
       <c r="B7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
@@ -1082,7 +1062,7 @@
         <v>900230000088083</v>
       </c>
       <c r="C8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -1090,10 +1070,10 @@
         <v>900230000087402</v>
       </c>
       <c r="B9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
@@ -1101,10 +1081,10 @@
         <v>900230000087403</v>
       </c>
       <c r="B10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
@@ -1112,7 +1092,7 @@
         <v>900230000088082</v>
       </c>
       <c r="C11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
@@ -1120,7 +1100,7 @@
         <v>900230000228791</v>
       </c>
       <c r="C12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
@@ -1128,7 +1108,27 @@
         <v>900230000087401</v>
       </c>
       <c r="C13" t="s">
-        <v>46</v>
+        <v>45</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
slight variable name changes
</commit_message>
<xml_diff>
--- a/data/WGFP Metadata.xlsx
+++ b/data/WGFP Metadata.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072"/>
   </bookViews>
   <sheets>
     <sheet name="AntennaMetadata" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="77">
   <si>
     <t>Variable</t>
   </si>
@@ -44,15 +44,6 @@
     <t>StationingLocation</t>
   </si>
   <si>
-    <t>B4</t>
-  </si>
-  <si>
-    <t>B5</t>
-  </si>
-  <si>
-    <t>B6</t>
-  </si>
-  <si>
     <t>Fraser River Canyon</t>
   </si>
   <si>
@@ -179,9 +170,6 @@
     <t>SiteName</t>
   </si>
   <si>
-    <t>SiteCode</t>
-  </si>
-  <si>
     <t>River</t>
   </si>
   <si>
@@ -239,7 +227,37 @@
     <t xml:space="preserve">Connectivity Channel Downstream (Upstream) </t>
   </si>
   <si>
-    <t>WG3</t>
+    <t>GD1</t>
+  </si>
+  <si>
+    <t>B3</t>
+  </si>
+  <si>
+    <t>RR1</t>
+  </si>
+  <si>
+    <t>FC1</t>
+  </si>
+  <si>
+    <t>For the biomark antennas, I don't think you can actually input the readers to say the codes; only stuff like A4,B2 etc…</t>
+  </si>
+  <si>
+    <t>A1, B1</t>
+  </si>
+  <si>
+    <t>A2, B2</t>
+  </si>
+  <si>
+    <t>A3</t>
+  </si>
+  <si>
+    <t>A4</t>
+  </si>
+  <si>
+    <t>FrontendSiteCode</t>
+  </si>
+  <si>
+    <t>BackendSiteCode</t>
   </si>
 </sst>
 </file>
@@ -559,10 +577,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -570,362 +588,420 @@
     <col min="1" max="1" width="42.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="51.88671875" customWidth="1"/>
     <col min="3" max="3" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>1</v>
       </c>
       <c r="B1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D2" t="s">
+        <v>71</v>
+      </c>
+      <c r="E2">
+        <v>416026</v>
+      </c>
+      <c r="F2">
+        <v>4440196</v>
+      </c>
+      <c r="G2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D3" t="s">
+        <v>72</v>
+      </c>
+      <c r="E3">
+        <v>420728</v>
+      </c>
+      <c r="F3">
+        <v>4437221</v>
+      </c>
+      <c r="G3" t="s">
         <v>49</v>
       </c>
-      <c r="C1" t="s">
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C4" t="s">
+        <v>68</v>
+      </c>
+      <c r="D4" t="s">
+        <v>73</v>
+      </c>
+      <c r="E4">
+        <v>419210</v>
+      </c>
+      <c r="F4">
+        <v>4439961</v>
+      </c>
+      <c r="G4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C5" t="s">
+        <v>69</v>
+      </c>
+      <c r="D5" t="s">
+        <v>74</v>
+      </c>
+      <c r="E5">
+        <v>424543</v>
+      </c>
+      <c r="F5">
+        <v>4435559</v>
+      </c>
+      <c r="G5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" t="s">
+        <v>56</v>
+      </c>
+      <c r="C6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6">
+        <v>412489</v>
+      </c>
+      <c r="F6">
+        <v>4439413</v>
+      </c>
+      <c r="G6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
+        <v>56</v>
+      </c>
+      <c r="C7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7">
+        <v>412489</v>
+      </c>
+      <c r="F7" s="1">
+        <v>4439413</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" t="s">
+        <v>57</v>
+      </c>
+      <c r="C8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8">
+        <v>414375</v>
+      </c>
+      <c r="F8">
+        <v>4440241</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" t="s">
+        <v>57</v>
+      </c>
+      <c r="C9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9">
+        <v>414375</v>
+      </c>
+      <c r="F9">
+        <v>4440241</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" t="s">
+        <v>58</v>
+      </c>
+      <c r="C10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" t="s">
+        <v>18</v>
+      </c>
+      <c r="E10">
+        <v>416965</v>
+      </c>
+      <c r="F10">
+        <v>4439369</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" t="s">
+        <v>58</v>
+      </c>
+      <c r="C11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" t="s">
+        <v>19</v>
+      </c>
+      <c r="E11">
+        <v>416965</v>
+      </c>
+      <c r="F11">
+        <v>4439369</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" t="s">
+        <v>59</v>
+      </c>
+      <c r="C12" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" t="s">
+        <v>21</v>
+      </c>
+      <c r="E12">
+        <v>415802</v>
+      </c>
+      <c r="F12">
+        <v>4439907</v>
+      </c>
+      <c r="G12" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B2" t="s">
-        <v>56</v>
-      </c>
-      <c r="C2" t="s">
-        <v>70</v>
-      </c>
-      <c r="D2">
-        <v>416026</v>
-      </c>
-      <c r="E2">
-        <v>4440196</v>
-      </c>
-      <c r="F2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" t="s">
-        <v>57</v>
-      </c>
-      <c r="C3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3">
-        <v>420728</v>
-      </c>
-      <c r="E3">
-        <v>4437221</v>
-      </c>
-      <c r="F3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" t="s">
-        <v>58</v>
-      </c>
-      <c r="C4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4">
-        <v>419210</v>
-      </c>
-      <c r="E4">
-        <v>4439961</v>
-      </c>
-      <c r="F4" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" t="s">
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>65</v>
+      </c>
+      <c r="B13" t="s">
         <v>59</v>
       </c>
-      <c r="C5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5">
-        <v>424543</v>
-      </c>
-      <c r="E5">
-        <v>4435559</v>
-      </c>
-      <c r="F5" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" t="s">
+      <c r="C13" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" t="s">
+        <v>22</v>
+      </c>
+      <c r="E13">
+        <v>415802</v>
+      </c>
+      <c r="F13">
+        <v>4439907</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" t="s">
         <v>60</v>
       </c>
-      <c r="C6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6">
-        <v>412489</v>
-      </c>
-      <c r="E6">
-        <v>4439413</v>
-      </c>
-      <c r="F6" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7" t="s">
+      <c r="C14" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14" t="s">
+        <v>23</v>
+      </c>
+      <c r="E14">
+        <v>415787</v>
+      </c>
+      <c r="F14">
+        <v>4439908</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" t="s">
         <v>60</v>
       </c>
-      <c r="C7" t="s">
-        <v>12</v>
-      </c>
-      <c r="D7">
-        <v>412489</v>
-      </c>
-      <c r="E7" s="1">
-        <v>4439413</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" t="s">
+      <c r="C15" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" t="s">
+        <v>24</v>
+      </c>
+      <c r="E15">
+        <v>415787</v>
+      </c>
+      <c r="F15">
+        <v>4439908</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" t="s">
         <v>61</v>
       </c>
-      <c r="C8" t="s">
-        <v>19</v>
-      </c>
-      <c r="D8">
-        <v>414375</v>
-      </c>
-      <c r="E8">
-        <v>4440241</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" t="s">
+      <c r="C16" t="s">
+        <v>25</v>
+      </c>
+      <c r="D16" t="s">
+        <v>25</v>
+      </c>
+      <c r="E16">
+        <v>416723</v>
+      </c>
+      <c r="F16">
+        <v>4439443</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>30</v>
+      </c>
+      <c r="B17" t="s">
         <v>61</v>
       </c>
-      <c r="C9" t="s">
-        <v>20</v>
-      </c>
-      <c r="D9">
-        <v>414375</v>
-      </c>
-      <c r="E9">
-        <v>4440241</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>17</v>
-      </c>
-      <c r="B10" t="s">
+      <c r="C17" t="s">
+        <v>26</v>
+      </c>
+      <c r="D17" t="s">
+        <v>26</v>
+      </c>
+      <c r="E17">
+        <v>416723</v>
+      </c>
+      <c r="F17">
+        <v>4439443</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B18" t="s">
+        <v>64</v>
+      </c>
+      <c r="C18" t="s">
         <v>62</v>
       </c>
-      <c r="C10" t="s">
-        <v>21</v>
-      </c>
-      <c r="D10">
-        <v>416965</v>
-      </c>
-      <c r="E10">
-        <v>4439369</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11" t="s">
+      <c r="D18" t="s">
         <v>62</v>
       </c>
-      <c r="C11" t="s">
-        <v>22</v>
-      </c>
-      <c r="D11">
-        <v>416965</v>
-      </c>
-      <c r="E11">
-        <v>4439369</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>23</v>
-      </c>
-      <c r="B12" t="s">
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B19" t="s">
+        <v>64</v>
+      </c>
+      <c r="C19" t="s">
         <v>63</v>
       </c>
-      <c r="C12" t="s">
-        <v>24</v>
-      </c>
-      <c r="D12">
-        <v>415802</v>
-      </c>
-      <c r="E12">
-        <v>4439907</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>69</v>
-      </c>
-      <c r="B13" t="s">
+      <c r="D19" t="s">
         <v>63</v>
-      </c>
-      <c r="C13" t="s">
-        <v>25</v>
-      </c>
-      <c r="D13">
-        <v>415802</v>
-      </c>
-      <c r="E13">
-        <v>4439907</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>30</v>
-      </c>
-      <c r="B14" t="s">
-        <v>64</v>
-      </c>
-      <c r="C14" t="s">
-        <v>26</v>
-      </c>
-      <c r="D14">
-        <v>415787</v>
-      </c>
-      <c r="E14">
-        <v>4439908</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>31</v>
-      </c>
-      <c r="B15" t="s">
-        <v>64</v>
-      </c>
-      <c r="C15" t="s">
-        <v>27</v>
-      </c>
-      <c r="D15">
-        <v>415787</v>
-      </c>
-      <c r="E15">
-        <v>4439908</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>32</v>
-      </c>
-      <c r="B16" t="s">
-        <v>65</v>
-      </c>
-      <c r="C16" t="s">
-        <v>28</v>
-      </c>
-      <c r="D16">
-        <v>416723</v>
-      </c>
-      <c r="E16">
-        <v>4439443</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>33</v>
-      </c>
-      <c r="B17" t="s">
-        <v>65</v>
-      </c>
-      <c r="C17" t="s">
-        <v>29</v>
-      </c>
-      <c r="D17">
-        <v>416723</v>
-      </c>
-      <c r="E17">
-        <v>4439443</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B18" t="s">
-        <v>68</v>
-      </c>
-      <c r="C18" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B19" t="s">
-        <v>68</v>
-      </c>
-      <c r="C19" t="s">
-        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -958,7 +1034,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B2">
         <v>10120</v>
@@ -966,7 +1042,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B3">
         <v>8330</v>
@@ -981,7 +1057,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
@@ -994,13 +1070,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -1008,7 +1084,7 @@
         <v>900230000102751</v>
       </c>
       <c r="B2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -1016,7 +1092,7 @@
         <v>900226001581072</v>
       </c>
       <c r="B3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -1024,7 +1100,7 @@
         <v>900230000004000</v>
       </c>
       <c r="C4" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -1032,7 +1108,7 @@
         <v>900230000087405</v>
       </c>
       <c r="C5" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -1040,10 +1116,10 @@
         <v>900230000087408</v>
       </c>
       <c r="B6" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C6" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -1051,10 +1127,10 @@
         <v>900226001546996</v>
       </c>
       <c r="B7" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C7" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
@@ -1062,7 +1138,7 @@
         <v>900230000088083</v>
       </c>
       <c r="C8" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -1070,10 +1146,10 @@
         <v>900230000087402</v>
       </c>
       <c r="B9" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C9" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
@@ -1081,10 +1157,10 @@
         <v>900230000087403</v>
       </c>
       <c r="B10" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C10" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
@@ -1092,7 +1168,7 @@
         <v>900230000088082</v>
       </c>
       <c r="C11" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
@@ -1100,7 +1176,7 @@
         <v>900230000228791</v>
       </c>
       <c r="C12" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
@@ -1108,7 +1184,7 @@
         <v>900230000087401</v>
       </c>
       <c r="C13" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -1118,7 +1194,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -1128,7 +1204,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>55</v>
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
enabling site code changes in metadata file without changing code
</commit_message>
<xml_diff>
--- a/data/WGFP Metadata.xlsx
+++ b/data/WGFP Metadata.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="AntennaMetadata" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="78">
   <si>
     <t>Variable</t>
   </si>
@@ -239,9 +239,6 @@
     <t>FC1</t>
   </si>
   <si>
-    <t>For the biomark antennas, I don't think you can actually input the readers to say the codes; only stuff like A4,B2 etc…</t>
-  </si>
-  <si>
     <t>A1, B1</t>
   </si>
   <si>
@@ -258,6 +255,12 @@
   </si>
   <si>
     <t>BackendSiteCode</t>
+  </si>
+  <si>
+    <t>For the biomark antennas, I don't think you can actually code the readers to detect as the frontend codes; only codes like A4,B2 etc…</t>
+  </si>
+  <si>
+    <t>For antenna metadatea codes, the frontend code should only have 1 entry. It's ok for the biomark backend codes to have multiple entries, but not the stationary ones</t>
   </si>
 </sst>
 </file>
@@ -579,7 +582,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
@@ -599,10 +602,10 @@
         <v>46</v>
       </c>
       <c r="C1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D1" t="s">
         <v>75</v>
-      </c>
-      <c r="D1" t="s">
-        <v>76</v>
       </c>
       <c r="E1" t="s">
         <v>2</v>
@@ -625,7 +628,7 @@
         <v>67</v>
       </c>
       <c r="D2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E2">
         <v>416026</v>
@@ -648,7 +651,7 @@
         <v>66</v>
       </c>
       <c r="D3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E3">
         <v>420728</v>
@@ -671,7 +674,7 @@
         <v>68</v>
       </c>
       <c r="D4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E4">
         <v>419210</v>
@@ -694,7 +697,7 @@
         <v>69</v>
       </c>
       <c r="D5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E5">
         <v>424543</v>
@@ -1194,11 +1197,9 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -1209,7 +1210,12 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>70</v>
+        <v>76</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated test tag notes in metadata: no tags changed
</commit_message>
<xml_diff>
--- a/data/WGFP Metadata.xlsx
+++ b/data/WGFP Metadata.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="AntennaMetadata" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="82">
   <si>
     <t>Variable</t>
   </si>
@@ -149,9 +149,6 @@
     <t xml:space="preserve">45 detections 2023-5-18 at red barn only </t>
   </si>
   <si>
-    <t>Pit tag on stick</t>
-  </si>
-  <si>
     <t>24 detections; at RB on 10/7/2020, 7/27/2023 at confluence, again at red barn on 8/1/2023</t>
   </si>
   <si>
@@ -261,6 +258,21 @@
   </si>
   <si>
     <t>For antenna metadatea codes, the frontend code should only have 1 entry. It's ok for the biomark backend codes to have multiple entries, but not the stationary ones</t>
+  </si>
+  <si>
+    <t>PVC Stick, 32 mm tag</t>
+  </si>
+  <si>
+    <t>PVC Stick, 12 mm tag</t>
+  </si>
+  <si>
+    <t>Rubber Duck</t>
+  </si>
+  <si>
+    <t>Streamer test tag, 32 mm tag</t>
+  </si>
+  <si>
+    <t>Probably another fly pit tag</t>
   </si>
 </sst>
 </file>
@@ -599,13 +611,13 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D1" t="s">
         <v>74</v>
-      </c>
-      <c r="D1" t="s">
-        <v>75</v>
       </c>
       <c r="E1" t="s">
         <v>2</v>
@@ -614,7 +626,7 @@
         <v>3</v>
       </c>
       <c r="G1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -622,13 +634,13 @@
         <v>32</v>
       </c>
       <c r="B2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E2">
         <v>416026</v>
@@ -637,7 +649,7 @@
         <v>4440196</v>
       </c>
       <c r="G2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -645,13 +657,13 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E3">
         <v>420728</v>
@@ -660,7 +672,7 @@
         <v>4437221</v>
       </c>
       <c r="G3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -668,13 +680,13 @@
         <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E4">
         <v>419210</v>
@@ -683,7 +695,7 @@
         <v>4439961</v>
       </c>
       <c r="G4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -691,13 +703,13 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E5">
         <v>424543</v>
@@ -706,7 +718,7 @@
         <v>4435559</v>
       </c>
       <c r="G5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -714,7 +726,7 @@
         <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C6" t="s">
         <v>8</v>
@@ -729,7 +741,7 @@
         <v>4439413</v>
       </c>
       <c r="G6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -737,7 +749,7 @@
         <v>12</v>
       </c>
       <c r="B7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C7" t="s">
         <v>9</v>
@@ -752,7 +764,7 @@
         <v>4439413</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
@@ -760,7 +772,7 @@
         <v>10</v>
       </c>
       <c r="B8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C8" t="s">
         <v>16</v>
@@ -775,7 +787,7 @@
         <v>4440241</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
@@ -783,7 +795,7 @@
         <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C9" t="s">
         <v>17</v>
@@ -798,7 +810,7 @@
         <v>4440241</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
@@ -806,7 +818,7 @@
         <v>14</v>
       </c>
       <c r="B10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C10" t="s">
         <v>18</v>
@@ -821,7 +833,7 @@
         <v>4439369</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
@@ -829,7 +841,7 @@
         <v>15</v>
       </c>
       <c r="B11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C11" t="s">
         <v>19</v>
@@ -844,7 +856,7 @@
         <v>4439369</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
@@ -852,7 +864,7 @@
         <v>20</v>
       </c>
       <c r="B12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C12" t="s">
         <v>21</v>
@@ -867,15 +879,15 @@
         <v>4439907</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C13" t="s">
         <v>22</v>
@@ -890,7 +902,7 @@
         <v>4439907</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
@@ -898,7 +910,7 @@
         <v>27</v>
       </c>
       <c r="B14" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C14" t="s">
         <v>23</v>
@@ -913,7 +925,7 @@
         <v>4439908</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
@@ -921,7 +933,7 @@
         <v>28</v>
       </c>
       <c r="B15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C15" t="s">
         <v>24</v>
@@ -936,7 +948,7 @@
         <v>4439908</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
@@ -944,7 +956,7 @@
         <v>29</v>
       </c>
       <c r="B16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C16" t="s">
         <v>25</v>
@@ -959,7 +971,7 @@
         <v>4439443</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
@@ -967,7 +979,7 @@
         <v>30</v>
       </c>
       <c r="B17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C17" t="s">
         <v>26</v>
@@ -982,29 +994,29 @@
         <v>4439443</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C18" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D18" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C19" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D19" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -1060,13 +1072,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26.6640625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="44.88671875" style="2" customWidth="1"/>
     <col min="2" max="2" width="28.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="76.77734375" bestFit="1" customWidth="1"/>
   </cols>
@@ -1079,7 +1091,7 @@
         <v>34</v>
       </c>
       <c r="C1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -1087,7 +1099,7 @@
         <v>900230000102751</v>
       </c>
       <c r="B2" t="s">
-        <v>40</v>
+        <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -1095,23 +1107,29 @@
         <v>900226001581072</v>
       </c>
       <c r="B3" t="s">
-        <v>40</v>
+        <v>78</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>900230000004000</v>
       </c>
+      <c r="B4" t="s">
+        <v>79</v>
+      </c>
       <c r="C4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>900230000087405</v>
       </c>
+      <c r="B5" t="s">
+        <v>81</v>
+      </c>
       <c r="C5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -1149,10 +1167,10 @@
         <v>900230000087402</v>
       </c>
       <c r="B9" t="s">
-        <v>35</v>
+        <v>80</v>
       </c>
       <c r="C9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
@@ -1160,10 +1178,10 @@
         <v>900230000087403</v>
       </c>
       <c r="B10" t="s">
-        <v>35</v>
+        <v>81</v>
       </c>
       <c r="C10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
@@ -1178,16 +1196,22 @@
       <c r="A12" s="2">
         <v>900230000228791</v>
       </c>
+      <c r="B12" t="s">
+        <v>77</v>
+      </c>
       <c r="C12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>900230000087401</v>
       </c>
+      <c r="B13" t="s">
+        <v>81</v>
+      </c>
       <c r="C13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -1199,23 +1223,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
most test tags confirmed from eric
</commit_message>
<xml_diff>
--- a/data/WGFP Metadata.xlsx
+++ b/data/WGFP Metadata.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072"/>
   </bookViews>
   <sheets>
     <sheet name="AntennaMetadata" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="75">
   <si>
     <t>Variable</t>
   </si>
@@ -134,36 +134,9 @@
     <t>type</t>
   </si>
   <si>
-    <t>?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">shows up starting 2023-8-29 through 11-28 on all different different antennas </t>
-  </si>
-  <si>
-    <t>10/31 - 11/28</t>
-  </si>
-  <si>
-    <t>5 detections 2023-5-18 at hp4 and cf5, cf6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">45 detections 2023-5-18 at red barn only </t>
-  </si>
-  <si>
-    <t>24 detections; at RB on 10/7/2020, 7/27/2023 at confluence, again at red barn on 8/1/2023</t>
-  </si>
-  <si>
-    <t>55 detections in 2023: 6/6, 6/23. 7/25 at RB, CF and HP</t>
-  </si>
-  <si>
-    <t>4 detections on 2020-10-08 at CF</t>
-  </si>
-  <si>
     <t>notes</t>
   </si>
   <si>
-    <t>no detections</t>
-  </si>
-  <si>
     <t>SiteName</t>
   </si>
   <si>
@@ -227,9 +200,6 @@
     <t>GD1</t>
   </si>
   <si>
-    <t>B3</t>
-  </si>
-  <si>
     <t>RR1</t>
   </si>
   <si>
@@ -272,7 +242,16 @@
     <t>Streamer test tag, 32 mm tag</t>
   </si>
   <si>
-    <t>Probably another fly pit tag</t>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>WG1</t>
+  </si>
+  <si>
+    <t>WG2</t>
+  </si>
+  <si>
+    <t>cone head tag, 32 mm tag</t>
   </si>
 </sst>
 </file>
@@ -592,10 +571,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G19"/>
+  <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -606,18 +585,18 @@
     <col min="4" max="4" width="15.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="C1" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="D1" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="E1" t="s">
         <v>2</v>
@@ -626,21 +605,24 @@
         <v>3</v>
       </c>
       <c r="G1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+      <c r="H1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>32</v>
       </c>
       <c r="B2" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="C2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="D2" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="E2">
         <v>416026</v>
@@ -649,159 +631,153 @@
         <v>4440196</v>
       </c>
       <c r="G2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E3">
+        <v>416127.3</v>
+      </c>
+      <c r="F3">
+        <v>4440146</v>
+      </c>
+      <c r="G3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>6</v>
       </c>
-      <c r="B3" t="s">
-        <v>52</v>
-      </c>
-      <c r="C3" t="s">
-        <v>65</v>
-      </c>
-      <c r="D3" t="s">
-        <v>70</v>
-      </c>
-      <c r="E3">
+      <c r="B4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C4" t="s">
+        <v>56</v>
+      </c>
+      <c r="D4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E4">
         <v>420728</v>
       </c>
-      <c r="F3">
+      <c r="F4">
         <v>4437221</v>
       </c>
-      <c r="G3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="G4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>7</v>
       </c>
-      <c r="B4" t="s">
-        <v>53</v>
-      </c>
-      <c r="C4" t="s">
-        <v>67</v>
-      </c>
-      <c r="D4" t="s">
-        <v>71</v>
-      </c>
-      <c r="E4">
+      <c r="B5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C5" t="s">
+        <v>57</v>
+      </c>
+      <c r="D5" t="s">
+        <v>61</v>
+      </c>
+      <c r="E5">
         <v>419210</v>
       </c>
-      <c r="F4">
+      <c r="F5">
         <v>4439961</v>
       </c>
-      <c r="G4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="G5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>5</v>
       </c>
-      <c r="B5" t="s">
-        <v>54</v>
-      </c>
-      <c r="C5" t="s">
-        <v>68</v>
-      </c>
-      <c r="D5" t="s">
-        <v>72</v>
-      </c>
-      <c r="E5">
+      <c r="B6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C6" t="s">
+        <v>58</v>
+      </c>
+      <c r="D6" t="s">
+        <v>62</v>
+      </c>
+      <c r="E6">
         <v>424543</v>
       </c>
-      <c r="F5">
+      <c r="F6">
         <v>4435559</v>
       </c>
-      <c r="G5" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="G6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
         <v>11</v>
       </c>
-      <c r="B6" t="s">
-        <v>55</v>
-      </c>
-      <c r="C6" t="s">
+      <c r="B7" t="s">
+        <v>46</v>
+      </c>
+      <c r="C7" t="s">
         <v>8</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D7" t="s">
         <v>8</v>
-      </c>
-      <c r="E6">
-        <v>412489</v>
-      </c>
-      <c r="F6">
-        <v>4439413</v>
-      </c>
-      <c r="G6" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" t="s">
-        <v>55</v>
-      </c>
-      <c r="C7" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7" t="s">
-        <v>9</v>
       </c>
       <c r="E7">
         <v>412489</v>
       </c>
-      <c r="F7" s="1">
+      <c r="F7">
         <v>4439413</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="G7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" t="s">
+        <v>46</v>
+      </c>
+      <c r="C8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8">
+        <v>412489</v>
+      </c>
+      <c r="F8" s="1">
+        <v>4439413</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" t="s">
-        <v>56</v>
-      </c>
-      <c r="C8" t="s">
+      <c r="C9" t="s">
         <v>16</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D9" t="s">
         <v>16</v>
-      </c>
-      <c r="E8">
-        <v>414375</v>
-      </c>
-      <c r="F8">
-        <v>4440241</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9" t="s">
-        <v>56</v>
-      </c>
-      <c r="C9" t="s">
-        <v>17</v>
-      </c>
-      <c r="D9" t="s">
-        <v>17</v>
       </c>
       <c r="E9">
         <v>414375</v>
@@ -810,44 +786,44 @@
         <v>4440241</v>
       </c>
       <c r="G9" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+      <c r="C10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10">
+        <v>414375</v>
+      </c>
+      <c r="F10">
+        <v>4440241</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
         <v>14</v>
       </c>
-      <c r="B10" t="s">
-        <v>57</v>
-      </c>
-      <c r="C10" t="s">
+      <c r="B11" t="s">
+        <v>48</v>
+      </c>
+      <c r="C11" t="s">
         <v>18</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D11" t="s">
         <v>18</v>
-      </c>
-      <c r="E10">
-        <v>416965</v>
-      </c>
-      <c r="F10">
-        <v>4439369</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>15</v>
-      </c>
-      <c r="B11" t="s">
-        <v>57</v>
-      </c>
-      <c r="C11" t="s">
-        <v>19</v>
-      </c>
-      <c r="D11" t="s">
-        <v>19</v>
       </c>
       <c r="E11">
         <v>416965</v>
@@ -856,44 +832,44 @@
         <v>4439369</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" t="s">
+        <v>48</v>
+      </c>
+      <c r="C12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" t="s">
+        <v>19</v>
+      </c>
+      <c r="E12">
+        <v>416965</v>
+      </c>
+      <c r="F12">
+        <v>4439369</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
         <v>20</v>
       </c>
-      <c r="B12" t="s">
-        <v>58</v>
-      </c>
-      <c r="C12" t="s">
+      <c r="B13" t="s">
+        <v>49</v>
+      </c>
+      <c r="C13" t="s">
         <v>21</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D13" t="s">
         <v>21</v>
-      </c>
-      <c r="E12">
-        <v>415802</v>
-      </c>
-      <c r="F12">
-        <v>4439907</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>64</v>
-      </c>
-      <c r="B13" t="s">
-        <v>58</v>
-      </c>
-      <c r="C13" t="s">
-        <v>22</v>
-      </c>
-      <c r="D13" t="s">
-        <v>22</v>
       </c>
       <c r="E13">
         <v>415802</v>
@@ -902,44 +878,44 @@
         <v>4439907</v>
       </c>
       <c r="G13" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>55</v>
+      </c>
+      <c r="B14" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+      <c r="C14" t="s">
+        <v>22</v>
+      </c>
+      <c r="D14" t="s">
+        <v>22</v>
+      </c>
+      <c r="E14">
+        <v>415802</v>
+      </c>
+      <c r="F14">
+        <v>4439907</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
         <v>27</v>
       </c>
-      <c r="B14" t="s">
-        <v>59</v>
-      </c>
-      <c r="C14" t="s">
+      <c r="B15" t="s">
+        <v>50</v>
+      </c>
+      <c r="C15" t="s">
         <v>23</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D15" t="s">
         <v>23</v>
-      </c>
-      <c r="E14">
-        <v>415787</v>
-      </c>
-      <c r="F14">
-        <v>4439908</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>28</v>
-      </c>
-      <c r="B15" t="s">
-        <v>59</v>
-      </c>
-      <c r="C15" t="s">
-        <v>24</v>
-      </c>
-      <c r="D15" t="s">
-        <v>24</v>
       </c>
       <c r="E15">
         <v>415787</v>
@@ -948,44 +924,44 @@
         <v>4439908</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B16" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="C16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E16">
-        <v>416723</v>
+        <v>415787</v>
       </c>
       <c r="F16">
-        <v>4439443</v>
+        <v>4439908</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B17" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="C17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E17">
         <v>416723</v>
@@ -994,29 +970,52 @@
         <v>4439443</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>30</v>
+      </c>
       <c r="B18" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="C18" t="s">
-        <v>61</v>
+        <v>26</v>
       </c>
       <c r="D18" t="s">
-        <v>61</v>
+        <v>26</v>
+      </c>
+      <c r="E18">
+        <v>416723</v>
+      </c>
+      <c r="F18">
+        <v>4439443</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="C19" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="D19" t="s">
-        <v>62</v>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B20" t="s">
+        <v>54</v>
+      </c>
+      <c r="C20" t="s">
+        <v>53</v>
+      </c>
+      <c r="D20" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -1070,10 +1069,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1091,7 +1090,7 @@
         <v>34</v>
       </c>
       <c r="C1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -1099,7 +1098,7 @@
         <v>900230000102751</v>
       </c>
       <c r="B2" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -1107,7 +1106,7 @@
         <v>900226001581072</v>
       </c>
       <c r="B3" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -1115,10 +1114,7 @@
         <v>900230000004000</v>
       </c>
       <c r="B4" t="s">
-        <v>79</v>
-      </c>
-      <c r="C4" t="s">
-        <v>42</v>
+        <v>69</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -1126,10 +1122,7 @@
         <v>900230000087405</v>
       </c>
       <c r="B5" t="s">
-        <v>81</v>
-      </c>
-      <c r="C5" t="s">
-        <v>44</v>
+        <v>67</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -1137,10 +1130,7 @@
         <v>900230000087408</v>
       </c>
       <c r="B6" t="s">
-        <v>35</v>
-      </c>
-      <c r="C6" t="s">
-        <v>36</v>
+        <v>67</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -1148,18 +1138,15 @@
         <v>900226001546996</v>
       </c>
       <c r="B7" t="s">
-        <v>35</v>
-      </c>
-      <c r="C7" t="s">
-        <v>37</v>
+        <v>68</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>900230000088083</v>
       </c>
-      <c r="C8" t="s">
-        <v>38</v>
+      <c r="B8" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -1167,10 +1154,7 @@
         <v>900230000087402</v>
       </c>
       <c r="B9" t="s">
-        <v>80</v>
-      </c>
-      <c r="C9" t="s">
-        <v>44</v>
+        <v>74</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
@@ -1178,29 +1162,20 @@
         <v>900230000087403</v>
       </c>
       <c r="B10" t="s">
-        <v>81</v>
-      </c>
-      <c r="C10" t="s">
-        <v>44</v>
+        <v>74</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>900230000088082</v>
       </c>
-      <c r="C11" t="s">
-        <v>39</v>
-      </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>900230000228791</v>
       </c>
       <c r="B12" t="s">
-        <v>77</v>
-      </c>
-      <c r="C12" t="s">
-        <v>40</v>
+        <v>67</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
@@ -1208,10 +1183,15 @@
         <v>900230000087401</v>
       </c>
       <c r="B13" t="s">
-        <v>81</v>
-      </c>
-      <c r="C13" t="s">
-        <v>41</v>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="2">
+        <v>900230000088084</v>
+      </c>
+      <c r="B14" t="s">
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -1229,17 +1209,17 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Windy gap biomark (B3)  split to Bypass and auxiliary
</commit_message>
<xml_diff>
--- a/data/WGFP Metadata.xlsx
+++ b/data/WGFP Metadata.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="83">
   <si>
     <t>Variable</t>
   </si>
@@ -155,9 +155,6 @@
     <t>Assumes that for AntennaMetadata, SiteName and River will not be changing. If they do change, you'll have to go into the runscript and ac couple functions including "PrepareforMovementsStatesand Summaries" to change how those variabels are located</t>
   </si>
   <si>
-    <t>Windy Gap Dam Biomark Antenna</t>
-  </si>
-  <si>
     <t>Kaibab Park Biomark Antenna</t>
   </si>
   <si>
@@ -206,9 +203,6 @@
     <t>FC1</t>
   </si>
   <si>
-    <t>A1, B1</t>
-  </si>
-  <si>
     <t>A2, B2</t>
   </si>
   <si>
@@ -224,9 +218,6 @@
     <t>BackendSiteCode</t>
   </si>
   <si>
-    <t>For the biomark antennas, I don't think you can actually code the readers to detect as the frontend codes; only codes like A4,B2 etc…</t>
-  </si>
-  <si>
     <t>For antenna metadatea codes, the frontend code should only have 1 entry. It's ok for the biomark backend codes to have multiple entries, but not the stationary ones</t>
   </si>
   <si>
@@ -252,6 +243,39 @@
   </si>
   <si>
     <t>cone head tag, 32 mm tag</t>
+  </si>
+  <si>
+    <t>For the biomark antennas, I don't think you can actually code the readers to detect as the frontend codes; only codes like A4,B2 etc…hence the need for frotend/backend codes</t>
+  </si>
+  <si>
+    <t>For marker color to be assigned correctly, need to have "Biomark Antenna", "Stationary Antenna", and "Mobile Run" in SiteName</t>
+  </si>
+  <si>
+    <t>DeploymentDuration</t>
+  </si>
+  <si>
+    <t>Spring 2022 - Fall 2022</t>
+  </si>
+  <si>
+    <t>Spring 2021 - Fall 2021</t>
+  </si>
+  <si>
+    <t>B1</t>
+  </si>
+  <si>
+    <t>A1</t>
+  </si>
+  <si>
+    <t>Windy Gap Bypass Channel Biomark Antenna</t>
+  </si>
+  <si>
+    <t>Windy Gap Auxiliary Biomark Antenna</t>
+  </si>
+  <si>
+    <t>Windy Gap Bypass Channel</t>
+  </si>
+  <si>
+    <t>Windy Gap Auxiliary</t>
   </si>
 </sst>
 </file>
@@ -571,21 +595,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H20"/>
+  <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="42.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="51.88671875" customWidth="1"/>
-    <col min="3" max="3" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.77734375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -593,10 +618,10 @@
         <v>36</v>
       </c>
       <c r="C1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E1" t="s">
         <v>2</v>
@@ -608,21 +633,24 @@
         <v>37</v>
       </c>
       <c r="H1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+        <v>74</v>
+      </c>
+      <c r="I1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>32</v>
+        <v>81</v>
       </c>
       <c r="B2" t="s">
-        <v>42</v>
+        <v>79</v>
       </c>
       <c r="C2" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D2" t="s">
-        <v>59</v>
+        <v>77</v>
       </c>
       <c r="E2">
         <v>416026</v>
@@ -633,13 +661,22 @@
       <c r="G2" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B3" t="s">
+        <v>80</v>
+      </c>
       <c r="C3" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D3" t="s">
-        <v>59</v>
+        <v>78</v>
       </c>
       <c r="E3">
         <v>416127.3</v>
@@ -650,19 +687,22 @@
       <c r="G3" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E4">
         <v>420728</v>
@@ -674,18 +714,18 @@
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E5">
         <v>419210</v>
@@ -697,18 +737,18 @@
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D6" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E6">
         <v>424543</v>
@@ -720,12 +760,12 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C7" t="s">
         <v>8</v>
@@ -743,12 +783,12 @@
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C8" t="s">
         <v>9</v>
@@ -765,13 +805,14 @@
       <c r="G8" s="1" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H8" s="1"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C9" t="s">
         <v>16</v>
@@ -788,13 +829,14 @@
       <c r="G9" s="1" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H9" s="1"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>13</v>
       </c>
       <c r="B10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C10" t="s">
         <v>17</v>
@@ -811,13 +853,14 @@
       <c r="G10" s="1" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H10" s="1"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>14</v>
       </c>
       <c r="B11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C11" t="s">
         <v>18</v>
@@ -834,13 +877,14 @@
       <c r="G11" s="1" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H11" s="1"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>15</v>
       </c>
       <c r="B12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C12" t="s">
         <v>19</v>
@@ -857,13 +901,14 @@
       <c r="G12" s="1" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H12" s="1"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>20</v>
       </c>
       <c r="B13" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C13" t="s">
         <v>21</v>
@@ -880,13 +925,14 @@
       <c r="G13" s="1" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H13" s="1"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C14" t="s">
         <v>22</v>
@@ -903,13 +949,14 @@
       <c r="G14" s="1" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H14" s="1"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>27</v>
       </c>
       <c r="B15" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C15" t="s">
         <v>23</v>
@@ -926,13 +973,14 @@
       <c r="G15" s="1" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H15" s="1"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>28</v>
       </c>
       <c r="B16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C16" t="s">
         <v>24</v>
@@ -949,13 +997,14 @@
       <c r="G16" s="1" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H16" s="1"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>29</v>
       </c>
       <c r="B17" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C17" t="s">
         <v>25</v>
@@ -972,13 +1021,14 @@
       <c r="G17" s="1" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H17" s="1"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>30</v>
       </c>
       <c r="B18" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C18" t="s">
         <v>26</v>
@@ -995,27 +1045,28 @@
       <c r="G18" s="1" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H18" s="1"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C19" t="s">
+        <v>51</v>
+      </c>
+      <c r="D19" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B20" t="s">
+        <v>53</v>
+      </c>
+      <c r="C20" t="s">
         <v>52</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D20" t="s">
         <v>52</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B20" t="s">
-        <v>54</v>
-      </c>
-      <c r="C20" t="s">
-        <v>53</v>
-      </c>
-      <c r="D20" t="s">
-        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -1098,7 +1149,7 @@
         <v>900230000102751</v>
       </c>
       <c r="B2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -1106,7 +1157,7 @@
         <v>900226001581072</v>
       </c>
       <c r="B3" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -1114,7 +1165,7 @@
         <v>900230000004000</v>
       </c>
       <c r="B4" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -1122,7 +1173,7 @@
         <v>900230000087405</v>
       </c>
       <c r="B5" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -1130,7 +1181,7 @@
         <v>900230000087408</v>
       </c>
       <c r="B6" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -1138,7 +1189,7 @@
         <v>900226001546996</v>
       </c>
       <c r="B7" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
@@ -1146,7 +1197,7 @@
         <v>900230000088083</v>
       </c>
       <c r="B8" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -1154,7 +1205,7 @@
         <v>900230000087402</v>
       </c>
       <c r="B9" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
@@ -1162,7 +1213,7 @@
         <v>900230000087403</v>
       </c>
       <c r="B10" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
@@ -1175,7 +1226,7 @@
         <v>900230000228791</v>
       </c>
       <c r="B12" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
@@ -1183,7 +1234,7 @@
         <v>900230000087401</v>
       </c>
       <c r="B13" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
@@ -1191,7 +1242,7 @@
         <v>900230000088084</v>
       </c>
       <c r="B14" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -1201,9 +1252,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:A4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -1214,12 +1267,17 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>66</v>
+        <v>63</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
kaibab park transitioned to Grandy Diversion
</commit_message>
<xml_diff>
--- a/data/WGFP Metadata.xlsx
+++ b/data/WGFP Metadata.xlsx
@@ -47,9 +47,6 @@
     <t>Fraser River Canyon</t>
   </si>
   <si>
-    <t>Kaibab Park</t>
-  </si>
-  <si>
     <t>River Run</t>
   </si>
   <si>
@@ -155,9 +152,6 @@
     <t>Assumes that for AntennaMetadata, SiteName and River will not be changing. If they do change, you'll have to go into the runscript and ac couple functions including "PrepareforMovementsStatesand Summaries" to change how those variabels are located</t>
   </si>
   <si>
-    <t>Kaibab Park Biomark Antenna</t>
-  </si>
-  <si>
     <t>River Run Biomark Antenna</t>
   </si>
   <si>
@@ -276,6 +270,12 @@
   </si>
   <si>
     <t>Windy Gap Auxiliary</t>
+  </si>
+  <si>
+    <t>Granby Diversion</t>
+  </si>
+  <si>
+    <t>Granby Diversion Biomark Antenna</t>
   </si>
 </sst>
 </file>
@@ -598,7 +598,7 @@
   <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -615,13 +615,13 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E1" t="s">
         <v>2</v>
@@ -630,27 +630,27 @@
         <v>3</v>
       </c>
       <c r="G1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="I1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E2">
         <v>416026</v>
@@ -659,24 +659,24 @@
         <v>4440196</v>
       </c>
       <c r="G2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E3">
         <v>416127.3</v>
@@ -685,24 +685,24 @@
         <v>4440146</v>
       </c>
       <c r="G3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>81</v>
       </c>
       <c r="B4" t="s">
-        <v>42</v>
+        <v>82</v>
       </c>
       <c r="C4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E4">
         <v>420728</v>
@@ -711,21 +711,21 @@
         <v>4437221</v>
       </c>
       <c r="G4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E5">
         <v>419210</v>
@@ -734,7 +734,7 @@
         <v>4439961</v>
       </c>
       <c r="G5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
@@ -742,13 +742,13 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C6" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E6">
         <v>424543</v>
@@ -757,21 +757,21 @@
         <v>4435559</v>
       </c>
       <c r="G6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E7">
         <v>412489</v>
@@ -780,21 +780,21 @@
         <v>4439413</v>
       </c>
       <c r="G7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B8" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E8">
         <v>412489</v>
@@ -803,22 +803,22 @@
         <v>4439413</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H8" s="1"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E9">
         <v>414375</v>
@@ -827,22 +827,22 @@
         <v>4440241</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H9" s="1"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B10" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E10">
         <v>414375</v>
@@ -851,22 +851,22 @@
         <v>4440241</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H10" s="1"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B11" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E11">
         <v>416965</v>
@@ -875,22 +875,22 @@
         <v>4439369</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H11" s="1"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B12" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E12">
         <v>416965</v>
@@ -899,22 +899,22 @@
         <v>4439369</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H12" s="1"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" t="s">
+        <v>46</v>
+      </c>
+      <c r="C13" t="s">
         <v>20</v>
       </c>
-      <c r="B13" t="s">
-        <v>48</v>
-      </c>
-      <c r="C13" t="s">
-        <v>21</v>
-      </c>
       <c r="D13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E13">
         <v>415802</v>
@@ -923,22 +923,22 @@
         <v>4439907</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H13" s="1"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B14" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E14">
         <v>415802</v>
@@ -947,22 +947,22 @@
         <v>4439907</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H14" s="1"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B15" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E15">
         <v>415787</v>
@@ -971,22 +971,22 @@
         <v>4439908</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H15" s="1"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B16" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C16" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D16" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E16">
         <v>415787</v>
@@ -995,22 +995,22 @@
         <v>4439908</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H16" s="1"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B17" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E17">
         <v>416723</v>
@@ -1019,22 +1019,22 @@
         <v>4439443</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H17" s="1"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B18" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E18">
         <v>416723</v>
@@ -1043,30 +1043,30 @@
         <v>4439443</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H18" s="1"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C19" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D19" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C20" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D20" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -1099,7 +1099,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B2">
         <v>10120</v>
@@ -1107,7 +1107,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B3">
         <v>8330</v>
@@ -1135,13 +1135,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" t="s">
         <v>33</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>34</v>
-      </c>
-      <c r="C1" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -1149,7 +1149,7 @@
         <v>900230000102751</v>
       </c>
       <c r="B2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -1157,7 +1157,7 @@
         <v>900226001581072</v>
       </c>
       <c r="B3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -1165,7 +1165,7 @@
         <v>900230000004000</v>
       </c>
       <c r="B4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -1173,7 +1173,7 @@
         <v>900230000087405</v>
       </c>
       <c r="B5" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -1181,7 +1181,7 @@
         <v>900230000087408</v>
       </c>
       <c r="B6" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -1189,7 +1189,7 @@
         <v>900226001546996</v>
       </c>
       <c r="B7" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
@@ -1197,7 +1197,7 @@
         <v>900230000088083</v>
       </c>
       <c r="B8" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -1205,7 +1205,7 @@
         <v>900230000087402</v>
       </c>
       <c r="B9" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
@@ -1213,7 +1213,7 @@
         <v>900230000087403</v>
       </c>
       <c r="B10" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
@@ -1226,7 +1226,7 @@
         <v>900230000228791</v>
       </c>
       <c r="B12" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
@@ -1234,7 +1234,7 @@
         <v>900230000087401</v>
       </c>
       <c r="B13" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
@@ -1242,7 +1242,7 @@
         <v>900230000088084</v>
       </c>
       <c r="B14" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -1262,22 +1262,22 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new metadata and re-ran script
</commit_message>
<xml_diff>
--- a/data/WGFP Metadata.xlsx
+++ b/data/WGFP Metadata.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072"/>
   </bookViews>
   <sheets>
     <sheet name="AntennaMetadata" sheetId="1" r:id="rId1"/>
@@ -158,24 +158,6 @@
     <t>Fraser River Canyon Biomark Antenna</t>
   </si>
   <si>
-    <t>Red Barn Stationary Antenna</t>
-  </si>
-  <si>
-    <t>Hitching Post Stationary Antenna</t>
-  </si>
-  <si>
-    <t>Confluence Stationary Antenna</t>
-  </si>
-  <si>
-    <t>Connectivity Channel Downstream Stationary Antenna</t>
-  </si>
-  <si>
-    <t>Connectivity Channel Side Channel Stationary Antenna</t>
-  </si>
-  <si>
-    <t>Connectivity Channel Upstream Stationary Antenna</t>
-  </si>
-  <si>
     <t>M1</t>
   </si>
   <si>
@@ -279,6 +261,24 @@
   </si>
   <si>
     <t>first data date: 2020-08-06. detecitons before this date range</t>
+  </si>
+  <si>
+    <t>Red Barn</t>
+  </si>
+  <si>
+    <t>Hitching Post</t>
+  </si>
+  <si>
+    <t>Confluence</t>
+  </si>
+  <si>
+    <t>Connectivity Channel Downstream</t>
+  </si>
+  <si>
+    <t>Connectivity Channel Side Channel</t>
+  </si>
+  <si>
+    <t>Connectivity Channel Upstream</t>
   </si>
 </sst>
 </file>
@@ -600,8 +600,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -621,10 +621,10 @@
         <v>35</v>
       </c>
       <c r="C1" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="D1" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="E1" t="s">
         <v>2</v>
@@ -636,24 +636,24 @@
         <v>36</v>
       </c>
       <c r="H1" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="I1" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B2" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="C2" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="D2" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="E2">
         <v>416026</v>
@@ -665,21 +665,21 @@
         <v>37</v>
       </c>
       <c r="H2" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="B3" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="C3" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="D3" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="E3">
         <v>416127.3</v>
@@ -691,21 +691,21 @@
         <v>37</v>
       </c>
       <c r="H3" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="B4" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="C4" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="D4" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="E4">
         <v>420728</v>
@@ -725,10 +725,10 @@
         <v>41</v>
       </c>
       <c r="C5" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="D5" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="E5">
         <v>419210</v>
@@ -748,10 +748,10 @@
         <v>42</v>
       </c>
       <c r="C6" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="D6" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="E6">
         <v>424543</v>
@@ -768,7 +768,7 @@
         <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>43</v>
+        <v>78</v>
       </c>
       <c r="C7" t="s">
         <v>7</v>
@@ -791,7 +791,7 @@
         <v>11</v>
       </c>
       <c r="B8" t="s">
-        <v>43</v>
+        <v>78</v>
       </c>
       <c r="C8" t="s">
         <v>8</v>
@@ -815,7 +815,7 @@
         <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>44</v>
+        <v>79</v>
       </c>
       <c r="C9" t="s">
         <v>15</v>
@@ -839,7 +839,7 @@
         <v>12</v>
       </c>
       <c r="B10" t="s">
-        <v>44</v>
+        <v>79</v>
       </c>
       <c r="C10" t="s">
         <v>16</v>
@@ -863,7 +863,7 @@
         <v>13</v>
       </c>
       <c r="B11" t="s">
-        <v>45</v>
+        <v>80</v>
       </c>
       <c r="C11" t="s">
         <v>17</v>
@@ -887,7 +887,7 @@
         <v>14</v>
       </c>
       <c r="B12" t="s">
-        <v>45</v>
+        <v>80</v>
       </c>
       <c r="C12" t="s">
         <v>18</v>
@@ -911,7 +911,7 @@
         <v>19</v>
       </c>
       <c r="B13" t="s">
-        <v>46</v>
+        <v>81</v>
       </c>
       <c r="C13" t="s">
         <v>20</v>
@@ -932,10 +932,10 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="B14" t="s">
-        <v>46</v>
+        <v>81</v>
       </c>
       <c r="C14" t="s">
         <v>21</v>
@@ -959,7 +959,7 @@
         <v>26</v>
       </c>
       <c r="B15" t="s">
-        <v>47</v>
+        <v>82</v>
       </c>
       <c r="C15" t="s">
         <v>22</v>
@@ -983,7 +983,7 @@
         <v>27</v>
       </c>
       <c r="B16" t="s">
-        <v>47</v>
+        <v>82</v>
       </c>
       <c r="C16" t="s">
         <v>23</v>
@@ -1007,7 +1007,7 @@
         <v>28</v>
       </c>
       <c r="B17" t="s">
-        <v>48</v>
+        <v>83</v>
       </c>
       <c r="C17" t="s">
         <v>24</v>
@@ -1031,7 +1031,7 @@
         <v>29</v>
       </c>
       <c r="B18" t="s">
-        <v>48</v>
+        <v>83</v>
       </c>
       <c r="C18" t="s">
         <v>25</v>
@@ -1052,24 +1052,24 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="C19" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="D19" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="C20" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="D20" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -1125,7 +1125,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
@@ -1152,7 +1152,7 @@
         <v>900230000102751</v>
       </c>
       <c r="B2" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -1160,7 +1160,7 @@
         <v>900226001581072</v>
       </c>
       <c r="B3" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -1168,7 +1168,7 @@
         <v>900230000004000</v>
       </c>
       <c r="B4" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -1176,7 +1176,7 @@
         <v>900230000087405</v>
       </c>
       <c r="B5" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -1184,7 +1184,7 @@
         <v>900230000087408</v>
       </c>
       <c r="B6" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -1192,7 +1192,7 @@
         <v>900226001546996</v>
       </c>
       <c r="B7" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
@@ -1200,7 +1200,7 @@
         <v>900230000088083</v>
       </c>
       <c r="B8" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -1208,7 +1208,7 @@
         <v>900230000087402</v>
       </c>
       <c r="B9" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
@@ -1216,7 +1216,7 @@
         <v>900230000087403</v>
       </c>
       <c r="B10" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
@@ -1229,7 +1229,7 @@
         <v>900230000228791</v>
       </c>
       <c r="B12" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
@@ -1237,7 +1237,7 @@
         <v>900230000087401</v>
       </c>
       <c r="B13" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
@@ -1245,7 +1245,7 @@
         <v>900230000088084</v>
       </c>
       <c r="B14" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -1270,22 +1270,22 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changed metaData BACK and found missing rows in adding the funciton
forgot i shouldn;t change that metadata field and also now though I have 3 more rows than i should. I have no idea where they came from
</commit_message>
<xml_diff>
--- a/data/WGFP Metadata.xlsx
+++ b/data/WGFP Metadata.xlsx
@@ -263,22 +263,22 @@
     <t>first data date: 2020-08-06. detecitons before this date range</t>
   </si>
   <si>
-    <t>Red Barn</t>
-  </si>
-  <si>
-    <t>Hitching Post</t>
-  </si>
-  <si>
-    <t>Confluence</t>
-  </si>
-  <si>
-    <t>Connectivity Channel Downstream</t>
-  </si>
-  <si>
-    <t>Connectivity Channel Side Channel</t>
-  </si>
-  <si>
-    <t>Connectivity Channel Upstream</t>
+    <t>Red Barn Stationary Antenna</t>
+  </si>
+  <si>
+    <t>Hitching Post Stationary Antenna</t>
+  </si>
+  <si>
+    <t>Confluence Stationary Antenna</t>
+  </si>
+  <si>
+    <t>Connectivity Channel Downstream Stationary Antenna</t>
+  </si>
+  <si>
+    <t>Connectivity Channel Side Channel Stationary Antenna</t>
+  </si>
+  <si>
+    <t>Connectivity Channel Upstream Stationary Antenna</t>
   </si>
 </sst>
 </file>
@@ -601,7 +601,7 @@
   <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
added metadata colunm for PT name
</commit_message>
<xml_diff>
--- a/data/WGFP Metadata.xlsx
+++ b/data/WGFP Metadata.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="88">
   <si>
     <t>Variable</t>
   </si>
@@ -279,6 +279,18 @@
   </si>
   <si>
     <t>Connectivity Channel Upstream Stationary Antenna</t>
+  </si>
+  <si>
+    <t>PressureTransducerSiteName</t>
+  </si>
+  <si>
+    <t>Red Barn</t>
+  </si>
+  <si>
+    <t>Hitching Post</t>
+  </si>
+  <si>
+    <t>Confluence</t>
   </si>
 </sst>
 </file>
@@ -598,10 +610,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I20"/>
+  <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -610,10 +622,11 @@
     <col min="2" max="2" width="51.88671875" customWidth="1"/>
     <col min="3" max="3" width="15.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.77734375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.77734375" customWidth="1"/>
+    <col min="9" max="9" width="19.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -627,22 +640,25 @@
         <v>54</v>
       </c>
       <c r="E1" t="s">
+        <v>84</v>
+      </c>
+      <c r="F1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>3</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>36</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>66</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>73</v>
       </c>
@@ -655,20 +671,20 @@
       <c r="D2" t="s">
         <v>69</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>416026</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>4440196</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>37</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>74</v>
       </c>
@@ -681,20 +697,20 @@
       <c r="D3" t="s">
         <v>70</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>416127.3</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>4440146</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>37</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>75</v>
       </c>
@@ -707,17 +723,17 @@
       <c r="D4" t="s">
         <v>50</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>420728</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>4437221</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -730,17 +746,17 @@
       <c r="D5" t="s">
         <v>51</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <v>419210</v>
       </c>
-      <c r="F5">
+      <c r="G5">
         <v>4439961</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -753,17 +769,17 @@
       <c r="D6" t="s">
         <v>52</v>
       </c>
-      <c r="E6">
+      <c r="F6">
         <v>424543</v>
       </c>
-      <c r="F6">
+      <c r="G6">
         <v>4435559</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -776,17 +792,20 @@
       <c r="D7" t="s">
         <v>7</v>
       </c>
-      <c r="E7">
+      <c r="E7" t="s">
+        <v>85</v>
+      </c>
+      <c r="F7">
         <v>412489</v>
       </c>
-      <c r="F7">
+      <c r="G7">
         <v>4439413</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -799,18 +818,21 @@
       <c r="D8" t="s">
         <v>8</v>
       </c>
-      <c r="E8">
+      <c r="E8" t="s">
+        <v>85</v>
+      </c>
+      <c r="F8">
         <v>412489</v>
       </c>
-      <c r="F8" s="1">
+      <c r="G8" s="1">
         <v>4439413</v>
       </c>
-      <c r="G8" s="1" t="s">
+      <c r="H8" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="H8" s="1"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I8" s="1"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -823,18 +845,21 @@
       <c r="D9" t="s">
         <v>15</v>
       </c>
-      <c r="E9">
+      <c r="E9" t="s">
+        <v>86</v>
+      </c>
+      <c r="F9">
         <v>414375</v>
       </c>
-      <c r="F9">
+      <c r="G9">
         <v>4440241</v>
       </c>
-      <c r="G9" s="1" t="s">
+      <c r="H9" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="H9" s="1"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I9" s="1"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -847,18 +872,21 @@
       <c r="D10" t="s">
         <v>16</v>
       </c>
-      <c r="E10">
+      <c r="E10" t="s">
+        <v>86</v>
+      </c>
+      <c r="F10">
         <v>414375</v>
       </c>
-      <c r="F10">
+      <c r="G10">
         <v>4440241</v>
       </c>
-      <c r="G10" s="1" t="s">
+      <c r="H10" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="H10" s="1"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I10" s="1"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -871,18 +899,21 @@
       <c r="D11" t="s">
         <v>17</v>
       </c>
-      <c r="E11">
+      <c r="E11" t="s">
+        <v>87</v>
+      </c>
+      <c r="F11">
         <v>416965</v>
       </c>
-      <c r="F11">
+      <c r="G11">
         <v>4439369</v>
       </c>
-      <c r="G11" s="1" t="s">
+      <c r="H11" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="H11" s="1"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I11" s="1"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -895,18 +926,21 @@
       <c r="D12" t="s">
         <v>18</v>
       </c>
-      <c r="E12">
+      <c r="E12" t="s">
+        <v>87</v>
+      </c>
+      <c r="F12">
         <v>416965</v>
       </c>
-      <c r="F12">
+      <c r="G12">
         <v>4439369</v>
       </c>
-      <c r="G12" s="1" t="s">
+      <c r="H12" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="H12" s="1"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I12" s="1"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>19</v>
       </c>
@@ -919,18 +953,18 @@
       <c r="D13" t="s">
         <v>20</v>
       </c>
-      <c r="E13">
+      <c r="F13">
         <v>415802</v>
       </c>
-      <c r="F13">
+      <c r="G13">
         <v>4439907</v>
       </c>
-      <c r="G13" s="1" t="s">
+      <c r="H13" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="H13" s="1"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I13" s="1"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>46</v>
       </c>
@@ -943,18 +977,18 @@
       <c r="D14" t="s">
         <v>21</v>
       </c>
-      <c r="E14">
+      <c r="F14">
         <v>415802</v>
       </c>
-      <c r="F14">
+      <c r="G14">
         <v>4439907</v>
       </c>
-      <c r="G14" s="1" t="s">
+      <c r="H14" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="H14" s="1"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I14" s="1"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>26</v>
       </c>
@@ -967,18 +1001,18 @@
       <c r="D15" t="s">
         <v>22</v>
       </c>
-      <c r="E15">
+      <c r="F15">
         <v>415787</v>
       </c>
-      <c r="F15">
+      <c r="G15">
         <v>4439908</v>
       </c>
-      <c r="G15" s="1" t="s">
+      <c r="H15" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="H15" s="1"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I15" s="1"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>27</v>
       </c>
@@ -991,18 +1025,18 @@
       <c r="D16" t="s">
         <v>23</v>
       </c>
-      <c r="E16">
+      <c r="F16">
         <v>415787</v>
       </c>
-      <c r="F16">
+      <c r="G16">
         <v>4439908</v>
       </c>
-      <c r="G16" s="1" t="s">
+      <c r="H16" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="H16" s="1"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I16" s="1"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>28</v>
       </c>
@@ -1015,18 +1049,18 @@
       <c r="D17" t="s">
         <v>24</v>
       </c>
-      <c r="E17">
+      <c r="F17">
         <v>416723</v>
       </c>
-      <c r="F17">
+      <c r="G17">
         <v>4439443</v>
       </c>
-      <c r="G17" s="1" t="s">
+      <c r="H17" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="H17" s="1"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I17" s="1"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>29</v>
       </c>
@@ -1039,18 +1073,18 @@
       <c r="D18" t="s">
         <v>25</v>
       </c>
-      <c r="E18">
+      <c r="F18">
         <v>416723</v>
       </c>
-      <c r="F18">
+      <c r="G18">
         <v>4439443</v>
       </c>
-      <c r="G18" s="1" t="s">
+      <c r="H18" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="H18" s="1"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I18" s="1"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
         <v>45</v>
       </c>
@@ -1061,7 +1095,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
         <v>45</v>
       </c>

</xml_diff>

<commit_message>
added speed column meters per second
</commit_message>
<xml_diff>
--- a/data/WGFP Metadata.xlsx
+++ b/data/WGFP Metadata.xlsx
@@ -612,8 +612,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1053,7 +1053,7 @@
         <v>416723</v>
       </c>
       <c r="G17">
-        <v>4439443</v>
+        <v>4439438</v>
       </c>
       <c r="H17" s="1" t="s">
         <v>39</v>
@@ -1077,7 +1077,7 @@
         <v>416723</v>
       </c>
       <c r="G18">
-        <v>4439443</v>
+        <v>4439438</v>
       </c>
       <c r="H18" s="1" t="s">
         <v>39</v>

</xml_diff>

<commit_message>
starting on different sites for marker tag cataloguing, bring D distance
</commit_message>
<xml_diff>
--- a/data/WGFP Metadata.xlsx
+++ b/data/WGFP Metadata.xlsx
@@ -9,13 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="AntennaMetadata" sheetId="1" r:id="rId1"/>
     <sheet name="ImportantStationingVariables" sheetId="2" r:id="rId2"/>
     <sheet name="TestTags" sheetId="3" r:id="rId3"/>
-    <sheet name="Notes" sheetId="4" r:id="rId4"/>
+    <sheet name="MarkerTagIssues" sheetId="5" r:id="rId4"/>
+    <sheet name="Notes" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="97">
   <si>
     <t>Variable</t>
   </si>
@@ -291,6 +292,33 @@
   </si>
   <si>
     <t>Confluence</t>
+  </si>
+  <si>
+    <t>Site</t>
+  </si>
+  <si>
+    <t>TagNumber</t>
+  </si>
+  <si>
+    <t>Explanation</t>
+  </si>
+  <si>
+    <t>IssueEndDatetime</t>
+  </si>
+  <si>
+    <t>IssueStartDatetime</t>
+  </si>
+  <si>
+    <t>If I remember correclty, it's possible that we didn't turn the antenna correctly/turn it back on after a tune. Resolved at next site visit</t>
+  </si>
+  <si>
+    <t>believe it ran out of batteries and we coulnd't get to it. Had some detections in october for some reason?</t>
+  </si>
+  <si>
+    <t>Next site visit hopefully</t>
+  </si>
+  <si>
+    <t>not sure</t>
   </si>
 </sst>
 </file>
@@ -326,10 +354,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -612,7 +641,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
@@ -1289,6 +1318,95 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.6640625" style="2" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="E1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="3">
+        <v>44201.541666666664</v>
+      </c>
+      <c r="C2" s="3">
+        <v>44229.536111111112</v>
+      </c>
+      <c r="D2" s="2">
+        <v>5394</v>
+      </c>
+      <c r="E2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="3">
+        <v>45059.11041666667</v>
+      </c>
+      <c r="C3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D3" s="2">
+        <v>5394</v>
+      </c>
+      <c r="E3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="3">
+        <v>44139.497893518521</v>
+      </c>
+      <c r="C4" s="3">
+        <v>44168.577337962961</v>
+      </c>
+      <c r="D4" s="2">
+        <v>2102</v>
+      </c>
+      <c r="E4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
all antenna marker tag issues catalogued
</commit_message>
<xml_diff>
--- a/data/WGFP Metadata.xlsx
+++ b/data/WGFP Metadata.xlsx
@@ -9,13 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="AntennaMetadata" sheetId="1" r:id="rId1"/>
-    <sheet name="ImportantStationingVariables" sheetId="2" r:id="rId2"/>
-    <sheet name="TestTags" sheetId="3" r:id="rId3"/>
-    <sheet name="MarkerTagIssues" sheetId="5" r:id="rId4"/>
+    <sheet name="MarkerTagIssues" sheetId="5" r:id="rId2"/>
+    <sheet name="ImportantStationingVariables" sheetId="2" r:id="rId3"/>
+    <sheet name="TestTags" sheetId="3" r:id="rId4"/>
     <sheet name="Notes" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="110">
   <si>
     <t>Variable</t>
   </si>
@@ -231,12 +231,6 @@
     <t>DeploymentDuration</t>
   </si>
   <si>
-    <t>Spring 2022 - Fall 2022</t>
-  </si>
-  <si>
-    <t>Spring 2021 - Fall 2021</t>
-  </si>
-  <si>
     <t>B1</t>
   </si>
   <si>
@@ -300,9 +294,6 @@
     <t>TagNumber</t>
   </si>
   <si>
-    <t>Explanation</t>
-  </si>
-  <si>
     <t>IssueEndDatetime</t>
   </si>
   <si>
@@ -319,6 +310,54 @@
   </si>
   <si>
     <t>not sure</t>
+  </si>
+  <si>
+    <t>sporadically seemed to have some detections during this period, but very inconsistent</t>
+  </si>
+  <si>
+    <t>5655-5665</t>
+  </si>
+  <si>
+    <t>start date is when detections dtropped out altogether but gtoa little more sporadic starting June 26</t>
+  </si>
+  <si>
+    <t>some sporadic missed detections from 9/5 until 9/19, consistent after that</t>
+  </si>
+  <si>
+    <t>probably antenna maintenance</t>
+  </si>
+  <si>
+    <t>Super sporadic detections between these dates</t>
+  </si>
+  <si>
+    <t>weird pattern between these timestamps of consistent detectionsfor 3 hours, then like 5 hours without any</t>
+  </si>
+  <si>
+    <t>marker tag was going off constantly so setting was changed</t>
+  </si>
+  <si>
+    <t>not sure if times off are from not being deployed or out of battery or what. Based off marker tags</t>
+  </si>
+  <si>
+    <t>between end date and 6/15, there were some missed detections but not many</t>
+  </si>
+  <si>
+    <t xml:space="preserve">antenna was off due to the site fuse issue </t>
+  </si>
+  <si>
+    <t>not sure if this period was a marker issue or antenna wasn't deployed these dates</t>
+  </si>
+  <si>
+    <t>8/31/2021  5:43:55 PM to 2021-11-04 13:15:23, and 2022-04-06 14:09:41 to 6/15/2022  11:49:09 AM, and 8/31/2022  3:54:17 PM to 2022-11-02 12:18:19</t>
+  </si>
+  <si>
+    <t>2022-04-21 12:44:27 to 2022-06-15 11:53:38, and 2022-08-30 17:48:25 to 2022-11-02 11:27:41</t>
+  </si>
+  <si>
+    <t>2021-08-31 16:29:52 to 2021-11-05 13:20:02</t>
+  </si>
+  <si>
+    <t>if I recall correclty I think it ran out of battery and we were just 3 days late in replacing</t>
   </si>
 </sst>
 </file>
@@ -641,8 +680,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J20"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -669,7 +708,7 @@
         <v>54</v>
       </c>
       <c r="E1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="F1" t="s">
         <v>2</v>
@@ -689,16 +728,16 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C2" t="s">
         <v>61</v>
       </c>
       <c r="D2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F2">
         <v>416026</v>
@@ -710,21 +749,21 @@
         <v>37</v>
       </c>
       <c r="I2" t="s">
-        <v>67</v>
+        <v>107</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C3" t="s">
         <v>62</v>
       </c>
       <c r="D3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F3">
         <v>416127.3</v>
@@ -736,15 +775,15 @@
         <v>37</v>
       </c>
       <c r="I3" t="s">
-        <v>68</v>
+        <v>108</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C4" t="s">
         <v>47</v>
@@ -760,6 +799,12 @@
       </c>
       <c r="H4" t="s">
         <v>38</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="J4" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
@@ -813,7 +858,7 @@
         <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C7" t="s">
         <v>7</v>
@@ -822,7 +867,7 @@
         <v>7</v>
       </c>
       <c r="E7" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F7">
         <v>412489</v>
@@ -839,7 +884,7 @@
         <v>11</v>
       </c>
       <c r="B8" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C8" t="s">
         <v>8</v>
@@ -848,7 +893,7 @@
         <v>8</v>
       </c>
       <c r="E8" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F8">
         <v>412489</v>
@@ -866,7 +911,7 @@
         <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C9" t="s">
         <v>15</v>
@@ -875,7 +920,7 @@
         <v>15</v>
       </c>
       <c r="E9" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="F9">
         <v>414375</v>
@@ -893,7 +938,7 @@
         <v>12</v>
       </c>
       <c r="B10" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C10" t="s">
         <v>16</v>
@@ -902,7 +947,7 @@
         <v>16</v>
       </c>
       <c r="E10" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="F10">
         <v>414375</v>
@@ -920,7 +965,7 @@
         <v>13</v>
       </c>
       <c r="B11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C11" t="s">
         <v>17</v>
@@ -929,7 +974,7 @@
         <v>17</v>
       </c>
       <c r="E11" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F11">
         <v>416965</v>
@@ -947,7 +992,7 @@
         <v>14</v>
       </c>
       <c r="B12" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C12" t="s">
         <v>18</v>
@@ -956,7 +1001,7 @@
         <v>18</v>
       </c>
       <c r="E12" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F12">
         <v>416965</v>
@@ -974,7 +1019,7 @@
         <v>19</v>
       </c>
       <c r="B13" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C13" t="s">
         <v>20</v>
@@ -998,7 +1043,7 @@
         <v>46</v>
       </c>
       <c r="B14" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C14" t="s">
         <v>21</v>
@@ -1022,7 +1067,7 @@
         <v>26</v>
       </c>
       <c r="B15" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C15" t="s">
         <v>22</v>
@@ -1046,7 +1091,7 @@
         <v>27</v>
       </c>
       <c r="B16" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C16" t="s">
         <v>23</v>
@@ -1070,7 +1115,7 @@
         <v>28</v>
       </c>
       <c r="B17" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C17" t="s">
         <v>24</v>
@@ -1094,7 +1139,7 @@
         <v>29</v>
       </c>
       <c r="B18" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C18" t="s">
         <v>25</v>
@@ -1142,6 +1187,547 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E32"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="D7" workbookViewId="0">
+      <selection activeCell="K19" sqref="K19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.109375" style="2" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="3">
+        <v>44201.541666666664</v>
+      </c>
+      <c r="C2" s="3">
+        <v>44229.536111111112</v>
+      </c>
+      <c r="D2" s="2">
+        <v>5394</v>
+      </c>
+      <c r="E2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="3">
+        <v>45059.11041666667</v>
+      </c>
+      <c r="C3" t="s">
+        <v>92</v>
+      </c>
+      <c r="D3" s="2">
+        <v>5394</v>
+      </c>
+      <c r="E3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="3">
+        <v>44139.497893518521</v>
+      </c>
+      <c r="C4" s="3">
+        <v>44168.577337962961</v>
+      </c>
+      <c r="D4" s="2">
+        <v>2102</v>
+      </c>
+      <c r="E4" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="3">
+        <v>44692.109884259262</v>
+      </c>
+      <c r="C5" s="3">
+        <v>44720.489178240743</v>
+      </c>
+      <c r="D5" s="2">
+        <v>5154</v>
+      </c>
+      <c r="E5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="3">
+        <v>45058.031064814815</v>
+      </c>
+      <c r="C6" s="3">
+        <v>44721.468078703707</v>
+      </c>
+      <c r="D6" s="2">
+        <v>5154</v>
+      </c>
+      <c r="E6" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="3">
+        <v>45103.701516203706</v>
+      </c>
+      <c r="C7" s="3">
+        <v>45188.560648148145</v>
+      </c>
+      <c r="D7" s="2">
+        <v>5154</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="3">
+        <v>44138.917303240742</v>
+      </c>
+      <c r="C8" s="3">
+        <v>44168.671481481484</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="3">
+        <v>44172.428414351853</v>
+      </c>
+      <c r="C9" s="3">
+        <v>44175.531712962962</v>
+      </c>
+      <c r="D9" s="2">
+        <v>5665</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="3">
+        <v>45108.714178240742</v>
+      </c>
+      <c r="C10" s="3">
+        <v>45139.501180555555</v>
+      </c>
+      <c r="D10" s="2">
+        <v>5665</v>
+      </c>
+      <c r="E10" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="3">
+        <v>44625.756180555552</v>
+      </c>
+      <c r="C11" s="3">
+        <v>44648.585555555554</v>
+      </c>
+      <c r="D11" s="2">
+        <v>1570</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" s="3">
+        <v>44702.205983796295</v>
+      </c>
+      <c r="C12" s="3">
+        <v>44782.463171296295</v>
+      </c>
+      <c r="D12" s="2">
+        <v>1570</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" s="3">
+        <v>45097.797824074078</v>
+      </c>
+      <c r="C13" s="3">
+        <v>45174.730798611112</v>
+      </c>
+      <c r="D13" s="2">
+        <v>1570</v>
+      </c>
+      <c r="E13" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" s="3">
+        <v>45187.601886574077</v>
+      </c>
+      <c r="C14" s="3">
+        <v>45188.598344907405</v>
+      </c>
+      <c r="D14" s="2">
+        <v>1570</v>
+      </c>
+      <c r="E14" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" s="3">
+        <v>45187.59988425926</v>
+      </c>
+      <c r="C15" s="3">
+        <v>45188.602893518517</v>
+      </c>
+      <c r="D15" s="2">
+        <v>5396</v>
+      </c>
+      <c r="E15" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16" s="3">
+        <v>44700.45988425926</v>
+      </c>
+      <c r="C16" s="3">
+        <v>44700.904467592591</v>
+      </c>
+      <c r="D16" s="2">
+        <v>5396</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" s="3">
+        <v>44385.217766203707</v>
+      </c>
+      <c r="C17" s="3">
+        <v>44385.972615740742</v>
+      </c>
+      <c r="D17" s="2">
+        <v>5396</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" s="3">
+        <v>44727.209583333337</v>
+      </c>
+      <c r="C18" s="3">
+        <v>44742.85365740741</v>
+      </c>
+      <c r="D18" s="2">
+        <v>5396</v>
+      </c>
+      <c r="E18" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19" s="3">
+        <v>45227.74181712963</v>
+      </c>
+      <c r="C19" s="3">
+        <v>45239.424745370372</v>
+      </c>
+      <c r="D19" s="2">
+        <v>4948</v>
+      </c>
+      <c r="E19" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20" s="3">
+        <v>45318.982141203705</v>
+      </c>
+      <c r="C20" s="3">
+        <v>45335.619444444441</v>
+      </c>
+      <c r="D20" s="2">
+        <v>4948</v>
+      </c>
+      <c r="E20" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>21</v>
+      </c>
+      <c r="B21" s="3">
+        <v>45227.493541666663</v>
+      </c>
+      <c r="C21" s="3">
+        <v>45239.409525462965</v>
+      </c>
+      <c r="D21" s="2">
+        <v>2323</v>
+      </c>
+      <c r="E21" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>21</v>
+      </c>
+      <c r="B22" s="3">
+        <v>45318.978842592594</v>
+      </c>
+      <c r="C22" s="3">
+        <v>45335.639108796298</v>
+      </c>
+      <c r="D22" s="2">
+        <v>2323</v>
+      </c>
+      <c r="E22" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>22</v>
+      </c>
+      <c r="B23" s="3">
+        <v>45227.743541666663</v>
+      </c>
+      <c r="C23" s="3">
+        <v>45239.423483796294</v>
+      </c>
+      <c r="D23" s="2">
+        <v>12626</v>
+      </c>
+      <c r="E23" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>22</v>
+      </c>
+      <c r="B24" s="3">
+        <v>45318.976041666669</v>
+      </c>
+      <c r="C24" s="3">
+        <v>45335.627141203702</v>
+      </c>
+      <c r="D24" s="2">
+        <v>12626</v>
+      </c>
+      <c r="E24" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>23</v>
+      </c>
+      <c r="B25" s="3">
+        <v>45227.73877314815</v>
+      </c>
+      <c r="C25" s="3">
+        <v>45239.426585648151</v>
+      </c>
+      <c r="D25" s="2">
+        <v>4372</v>
+      </c>
+      <c r="E25" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>23</v>
+      </c>
+      <c r="B26" s="3">
+        <v>45318.97934027778</v>
+      </c>
+      <c r="C26" s="3">
+        <v>45335.637824074074</v>
+      </c>
+      <c r="D26" s="2">
+        <v>4372</v>
+      </c>
+      <c r="E26" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>24</v>
+      </c>
+      <c r="B27" s="3">
+        <v>45285.351435185185</v>
+      </c>
+      <c r="C27" t="s">
+        <v>92</v>
+      </c>
+      <c r="D27" s="2">
+        <v>12437</v>
+      </c>
+      <c r="E27" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>47</v>
+      </c>
+      <c r="B28" s="3">
+        <v>44472.646284722221</v>
+      </c>
+      <c r="C28" s="3">
+        <v>44475.538240740738</v>
+      </c>
+      <c r="D28" s="2">
+        <v>999000000007586</v>
+      </c>
+      <c r="E28" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>47</v>
+      </c>
+      <c r="B29" s="3">
+        <v>44683.650914351849</v>
+      </c>
+      <c r="C29" s="3">
+        <v>44684.478449074071</v>
+      </c>
+      <c r="D29" s="2">
+        <v>999000000007602</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>47</v>
+      </c>
+      <c r="B30" s="3">
+        <v>44696.561377314814</v>
+      </c>
+      <c r="C30" s="3">
+        <v>44707.610266203701</v>
+      </c>
+      <c r="D30" s="2">
+        <v>999000000007602</v>
+      </c>
+      <c r="E30" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>47</v>
+      </c>
+      <c r="B31" s="3">
+        <v>44727.492465277777</v>
+      </c>
+      <c r="C31" s="3">
+        <v>44804.66269675926</v>
+      </c>
+      <c r="D31" s="2">
+        <v>999000000007602</v>
+      </c>
+      <c r="E31" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>62</v>
+      </c>
+      <c r="B32" s="3">
+        <v>44472.19568287037</v>
+      </c>
+      <c r="C32" s="3">
+        <v>44475.510555555556</v>
+      </c>
+      <c r="D32" s="2">
+        <v>999000000007585</v>
+      </c>
+      <c r="E32" t="s">
+        <v>109</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
@@ -1184,7 +1770,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C14"/>
   <sheetViews>
@@ -1316,95 +1902,6 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E4"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="2" max="2" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.6640625" style="2" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>88</v>
-      </c>
-      <c r="B1" t="s">
-        <v>92</v>
-      </c>
-      <c r="C1" t="s">
-        <v>91</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="E1" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="3">
-        <v>44201.541666666664</v>
-      </c>
-      <c r="C2" s="3">
-        <v>44229.536111111112</v>
-      </c>
-      <c r="D2" s="2">
-        <v>5394</v>
-      </c>
-      <c r="E2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="3">
-        <v>45059.11041666667</v>
-      </c>
-      <c r="C3" t="s">
-        <v>95</v>
-      </c>
-      <c r="D3" s="2">
-        <v>5394</v>
-      </c>
-      <c r="E3" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="3">
-        <v>44139.497893518521</v>
-      </c>
-      <c r="C4" s="3">
-        <v>44168.577337962961</v>
-      </c>
-      <c r="D4" s="2">
-        <v>2102</v>
-      </c>
-      <c r="E4" t="s">
-        <v>96</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A5"/>
@@ -1437,7 +1934,7 @@
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
summary raw frequency table added
</commit_message>
<xml_diff>
--- a/data/WGFP Metadata.xlsx
+++ b/data/WGFP Metadata.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="AntennaMetadata" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="122">
   <si>
     <t>Variable</t>
   </si>
@@ -303,24 +303,12 @@
     <t>If I remember correclty, it's possible that we didn't turn the antenna correctly/turn it back on after a tune. Resolved at next site visit</t>
   </si>
   <si>
-    <t>believe it ran out of batteries and we coulnd't get to it. Had some detections in october for some reason?</t>
-  </si>
-  <si>
-    <t>Next site visit hopefully</t>
-  </si>
-  <si>
-    <t>not sure</t>
-  </si>
-  <si>
     <t>sporadically seemed to have some detections during this period, but very inconsistent</t>
   </si>
   <si>
     <t>5655-5665</t>
   </si>
   <si>
-    <t>start date is when detections dtropped out altogether but gtoa little more sporadic starting June 26</t>
-  </si>
-  <si>
     <t>some sporadic missed detections from 9/5 until 9/19, consistent after that</t>
   </si>
   <si>
@@ -345,19 +333,67 @@
     <t xml:space="preserve">antenna was off due to the site fuse issue </t>
   </si>
   <si>
-    <t>not sure if this period was a marker issue or antenna wasn't deployed these dates</t>
-  </si>
-  <si>
-    <t>8/31/2021  5:43:55 PM to 2021-11-04 13:15:23, and 2022-04-06 14:09:41 to 6/15/2022  11:49:09 AM, and 8/31/2022  3:54:17 PM to 2022-11-02 12:18:19</t>
-  </si>
-  <si>
     <t>2022-04-21 12:44:27 to 2022-06-15 11:53:38, and 2022-08-30 17:48:25 to 2022-11-02 11:27:41</t>
   </si>
   <si>
     <t>2021-08-31 16:29:52 to 2021-11-05 13:20:02</t>
   </si>
   <si>
-    <t>if I recall correclty I think it ran out of battery and we were just 3 days late in replacing</t>
+    <t>Not deployed</t>
+  </si>
+  <si>
+    <t>2020-08-07 12:00:30 to present</t>
+  </si>
+  <si>
+    <t>2020-08-07 12:15:37 to present</t>
+  </si>
+  <si>
+    <t>2020-08-07 10:29:17 to present</t>
+  </si>
+  <si>
+    <t>2020-08-07 09:29:03 to present</t>
+  </si>
+  <si>
+    <t>2020-08-07 19:35:00 to present</t>
+  </si>
+  <si>
+    <t>2020-08-07 19:35:07 to present</t>
+  </si>
+  <si>
+    <t>2023-10-18 12:44:05  to present</t>
+  </si>
+  <si>
+    <t>2023-10-18 12:57:39  to present</t>
+  </si>
+  <si>
+    <t>2023-10-18 12:59:02  to present</t>
+  </si>
+  <si>
+    <t>2023-10-18 13:01:15  to present</t>
+  </si>
+  <si>
+    <t>2023-10-18 13:15:04  to present</t>
+  </si>
+  <si>
+    <t>2023-10-18 13:20:42  to present</t>
+  </si>
+  <si>
+    <t>2021-08-31 17:43:55 to 2021-11-04 13:15:23, and 2022-04-06 14:09:41 to 2022-06-15 11:49:09, and 2022-08-2022 15:54:17 to 2022-11-02 12:18:19</t>
+  </si>
+  <si>
+    <t>Will be resolved with Next site visit hopefully</t>
+  </si>
+  <si>
+    <t>believe it ran out of batteries and we couldn't get to it. Had some detections in october for some reason?</t>
+  </si>
+  <si>
+    <t>start date is when detections dropped out altogether but got a little more sporadic starting June 26</t>
+  </si>
+  <si>
+    <t>if I recall correctly I think it ran out of battery and we were just 3 days late in replacing</t>
+  </si>
+  <si>
+    <t>sporadic, missed about half of marker detections during this period</t>
   </si>
 </sst>
 </file>
@@ -680,8 +716,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J20"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -749,7 +785,7 @@
         <v>37</v>
       </c>
       <c r="I2" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
@@ -775,7 +811,7 @@
         <v>37</v>
       </c>
       <c r="I3" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
@@ -801,10 +837,10 @@
         <v>38</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>106</v>
+        <v>116</v>
       </c>
       <c r="J4" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
@@ -829,6 +865,9 @@
       <c r="H5" t="s">
         <v>37</v>
       </c>
+      <c r="I5" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
@@ -852,6 +891,9 @@
       <c r="H6" t="s">
         <v>38</v>
       </c>
+      <c r="I6" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
@@ -878,6 +920,9 @@
       <c r="H7" t="s">
         <v>37</v>
       </c>
+      <c r="I7" s="1" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
@@ -904,7 +949,9 @@
       <c r="H8" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="I8" s="1"/>
+      <c r="I8" s="1" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
@@ -931,7 +978,9 @@
       <c r="H9" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="I9" s="1"/>
+      <c r="I9" s="1" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
@@ -958,7 +1007,9 @@
       <c r="H10" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="I10" s="1"/>
+      <c r="I10" s="1" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
@@ -985,7 +1036,9 @@
       <c r="H11" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="I11" s="1"/>
+      <c r="I11" s="1" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
@@ -1012,7 +1065,9 @@
       <c r="H12" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="I12" s="1"/>
+      <c r="I12" s="1" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
@@ -1036,7 +1091,9 @@
       <c r="H13" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="I13" s="1"/>
+      <c r="I13" s="1" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
@@ -1060,7 +1117,9 @@
       <c r="H14" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="I14" s="1"/>
+      <c r="I14" s="1" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
@@ -1084,7 +1143,9 @@
       <c r="H15" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="I15" s="1"/>
+      <c r="I15" s="1" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
@@ -1108,7 +1169,9 @@
       <c r="H16" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="I16" s="1"/>
+      <c r="I16" s="1" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
@@ -1132,7 +1195,9 @@
       <c r="H17" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="I17" s="1"/>
+      <c r="I17" s="1" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
@@ -1156,7 +1221,9 @@
       <c r="H18" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="I18" s="1"/>
+      <c r="I18" s="1" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
@@ -1188,17 +1255,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E32"/>
+  <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D7" workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
@@ -1243,13 +1310,13 @@
         <v>45059.11041666667</v>
       </c>
       <c r="C3" t="s">
-        <v>92</v>
+        <v>117</v>
       </c>
       <c r="D3" s="2">
         <v>5394</v>
       </c>
       <c r="E3" t="s">
-        <v>91</v>
+        <v>118</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -1265,9 +1332,6 @@
       <c r="D4" s="2">
         <v>2102</v>
       </c>
-      <c r="E4" t="s">
-        <v>93</v>
-      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
@@ -1283,7 +1347,7 @@
         <v>5154</v>
       </c>
       <c r="E5" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -1291,16 +1355,16 @@
         <v>15</v>
       </c>
       <c r="B6" s="3">
-        <v>45058.031064814815</v>
+        <v>44898.596435185187</v>
       </c>
       <c r="C6" s="3">
-        <v>44721.468078703707</v>
+        <v>44907.47210648148</v>
       </c>
       <c r="D6" s="2">
         <v>5154</v>
       </c>
       <c r="E6" t="s">
-        <v>94</v>
+        <v>121</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -1308,27 +1372,30 @@
         <v>15</v>
       </c>
       <c r="B7" s="3">
-        <v>45103.701516203706</v>
+        <v>45058.031064814815</v>
       </c>
       <c r="C7" s="3">
-        <v>45188.560648148145</v>
+        <v>44721.468078703707</v>
       </c>
       <c r="D7" s="2">
         <v>5154</v>
       </c>
+      <c r="E7" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B8" s="3">
-        <v>44138.917303240742</v>
+        <v>45103.701516203706</v>
       </c>
       <c r="C8" s="3">
-        <v>44168.671481481484</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>95</v>
+        <v>45188.560648148145</v>
+      </c>
+      <c r="D8" s="2">
+        <v>5154</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -1336,13 +1403,13 @@
         <v>16</v>
       </c>
       <c r="B9" s="3">
-        <v>44172.428414351853</v>
+        <v>44138.917303240742</v>
       </c>
       <c r="C9" s="3">
-        <v>44175.531712962962</v>
-      </c>
-      <c r="D9" s="2">
-        <v>5665</v>
+        <v>44168.671481481484</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
@@ -1350,44 +1417,44 @@
         <v>16</v>
       </c>
       <c r="B10" s="3">
-        <v>45108.714178240742</v>
+        <v>44172.428414351853</v>
       </c>
       <c r="C10" s="3">
-        <v>45139.501180555555</v>
+        <v>44175.531712962962</v>
       </c>
       <c r="D10" s="2">
         <v>5665</v>
       </c>
-      <c r="E10" t="s">
-        <v>96</v>
-      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B11" s="3">
-        <v>44625.756180555552</v>
+        <v>44694.853194444448</v>
       </c>
       <c r="C11" s="3">
-        <v>44648.585555555554</v>
+        <v>44695.658020833333</v>
       </c>
       <c r="D11" s="2">
-        <v>1570</v>
+        <v>5665</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B12" s="3">
-        <v>44702.205983796295</v>
+        <v>45108.714178240742</v>
       </c>
       <c r="C12" s="3">
-        <v>44782.463171296295</v>
+        <v>45139.501180555555</v>
       </c>
       <c r="D12" s="2">
-        <v>1570</v>
+        <v>5665</v>
+      </c>
+      <c r="E12" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
@@ -1395,16 +1462,13 @@
         <v>17</v>
       </c>
       <c r="B13" s="3">
-        <v>45097.797824074078</v>
+        <v>44625.756180555552</v>
       </c>
       <c r="C13" s="3">
-        <v>45174.730798611112</v>
+        <v>44648.585555555554</v>
       </c>
       <c r="D13" s="2">
         <v>1570</v>
-      </c>
-      <c r="E13" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
@@ -1412,47 +1476,47 @@
         <v>17</v>
       </c>
       <c r="B14" s="3">
-        <v>45187.601886574077</v>
+        <v>44702.205983796295</v>
       </c>
       <c r="C14" s="3">
-        <v>45188.598344907405</v>
+        <v>44782.463171296295</v>
       </c>
       <c r="D14" s="2">
         <v>1570</v>
       </c>
-      <c r="E14" t="s">
-        <v>98</v>
-      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B15" s="3">
-        <v>45187.59988425926</v>
+        <v>45097.797824074078</v>
       </c>
       <c r="C15" s="3">
-        <v>45188.602893518517</v>
+        <v>45174.730798611112</v>
       </c>
       <c r="D15" s="2">
-        <v>5396</v>
+        <v>1570</v>
       </c>
       <c r="E15" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B16" s="3">
-        <v>44700.45988425926</v>
+        <v>45187.601886574077</v>
       </c>
       <c r="C16" s="3">
-        <v>44700.904467592591</v>
+        <v>45188.598344907405</v>
       </c>
       <c r="D16" s="2">
-        <v>5396</v>
+        <v>1570</v>
+      </c>
+      <c r="E16" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
@@ -1460,13 +1524,16 @@
         <v>18</v>
       </c>
       <c r="B17" s="3">
-        <v>44385.217766203707</v>
+        <v>45187.59988425926</v>
       </c>
       <c r="C17" s="3">
-        <v>44385.972615740742</v>
+        <v>45188.602893518517</v>
       </c>
       <c r="D17" s="2">
         <v>5396</v>
+      </c>
+      <c r="E17" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
@@ -1474,200 +1541,197 @@
         <v>18</v>
       </c>
       <c r="B18" s="3">
-        <v>44727.209583333337</v>
+        <v>44700.45988425926</v>
       </c>
       <c r="C18" s="3">
-        <v>44742.85365740741</v>
+        <v>44700.904467592591</v>
       </c>
       <c r="D18" s="2">
         <v>5396</v>
       </c>
-      <c r="E18" t="s">
-        <v>99</v>
-      </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B19" s="3">
-        <v>45227.74181712963</v>
+        <v>44385.217766203707</v>
       </c>
       <c r="C19" s="3">
-        <v>45239.424745370372</v>
+        <v>44385.972615740742</v>
       </c>
       <c r="D19" s="2">
-        <v>4948</v>
-      </c>
-      <c r="E19" t="s">
-        <v>100</v>
+        <v>5396</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B20" s="3">
-        <v>45318.982141203705</v>
+        <v>44727.209583333337</v>
       </c>
       <c r="C20" s="3">
-        <v>45335.619444444441</v>
+        <v>44742.85365740741</v>
       </c>
       <c r="D20" s="2">
-        <v>4948</v>
+        <v>5396</v>
       </c>
       <c r="E20" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B21" s="3">
-        <v>45227.493541666663</v>
+        <v>45227.74181712963</v>
       </c>
       <c r="C21" s="3">
-        <v>45239.409525462965</v>
+        <v>45239.424745370372</v>
       </c>
       <c r="D21" s="2">
-        <v>2323</v>
+        <v>4948</v>
       </c>
       <c r="E21" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B22" s="3">
-        <v>45318.978842592594</v>
+        <v>45318.982141203705</v>
       </c>
       <c r="C22" s="3">
-        <v>45335.639108796298</v>
+        <v>45335.619444444441</v>
       </c>
       <c r="D22" s="2">
-        <v>2323</v>
+        <v>4948</v>
       </c>
       <c r="E22" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B23" s="3">
-        <v>45227.743541666663</v>
+        <v>45227.493541666663</v>
       </c>
       <c r="C23" s="3">
-        <v>45239.423483796294</v>
+        <v>45239.409525462965</v>
       </c>
       <c r="D23" s="2">
-        <v>12626</v>
+        <v>2323</v>
       </c>
       <c r="E23" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B24" s="3">
-        <v>45318.976041666669</v>
+        <v>45318.978842592594</v>
       </c>
       <c r="C24" s="3">
-        <v>45335.627141203702</v>
+        <v>45335.639108796298</v>
       </c>
       <c r="D24" s="2">
-        <v>12626</v>
+        <v>2323</v>
       </c>
       <c r="E24" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B25" s="3">
-        <v>45227.73877314815</v>
+        <v>45227.743541666663</v>
       </c>
       <c r="C25" s="3">
-        <v>45239.426585648151</v>
+        <v>45239.423483796294</v>
       </c>
       <c r="D25" s="2">
-        <v>4372</v>
+        <v>12626</v>
       </c>
       <c r="E25" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B26" s="3">
-        <v>45318.97934027778</v>
+        <v>45318.976041666669</v>
       </c>
       <c r="C26" s="3">
-        <v>45335.637824074074</v>
+        <v>45335.627141203702</v>
       </c>
       <c r="D26" s="2">
-        <v>4372</v>
+        <v>12626</v>
       </c>
       <c r="E26" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B27" s="3">
-        <v>45285.351435185185</v>
-      </c>
-      <c r="C27" t="s">
-        <v>92</v>
+        <v>45227.73877314815</v>
+      </c>
+      <c r="C27" s="3">
+        <v>45239.426585648151</v>
       </c>
       <c r="D27" s="2">
-        <v>12437</v>
+        <v>4372</v>
       </c>
       <c r="E27" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>47</v>
+        <v>23</v>
       </c>
       <c r="B28" s="3">
-        <v>44472.646284722221</v>
+        <v>45318.97934027778</v>
       </c>
       <c r="C28" s="3">
-        <v>44475.538240740738</v>
+        <v>45335.637824074074</v>
       </c>
       <c r="D28" s="2">
-        <v>999000000007586</v>
+        <v>4372</v>
       </c>
       <c r="E28" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>47</v>
+        <v>24</v>
       </c>
       <c r="B29" s="3">
-        <v>44683.650914351849</v>
-      </c>
-      <c r="C29" s="3">
-        <v>44684.478449074071</v>
+        <v>45285.351435185185</v>
+      </c>
+      <c r="C29" t="s">
+        <v>117</v>
       </c>
       <c r="D29" s="2">
-        <v>999000000007602</v>
+        <v>12437</v>
+      </c>
+      <c r="E29" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
@@ -1675,16 +1739,16 @@
         <v>47</v>
       </c>
       <c r="B30" s="3">
-        <v>44696.561377314814</v>
+        <v>44472.646284722221</v>
       </c>
       <c r="C30" s="3">
-        <v>44707.610266203701</v>
+        <v>44475.538240740738</v>
       </c>
       <c r="D30" s="2">
-        <v>999000000007602</v>
+        <v>999000000007586</v>
       </c>
       <c r="E30" t="s">
-        <v>103</v>
+        <v>120</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
@@ -1692,33 +1756,47 @@
         <v>47</v>
       </c>
       <c r="B31" s="3">
-        <v>44727.492465277777</v>
+        <v>44683.650914351849</v>
       </c>
       <c r="C31" s="3">
-        <v>44804.66269675926</v>
+        <v>44684.478449074071</v>
       </c>
       <c r="D31" s="2">
         <v>999000000007602</v>
       </c>
-      <c r="E31" t="s">
-        <v>105</v>
-      </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
+        <v>47</v>
+      </c>
+      <c r="B32" s="3">
+        <v>44696.561377314814</v>
+      </c>
+      <c r="C32" s="3">
+        <v>44707.610266203701</v>
+      </c>
+      <c r="D32" s="2">
+        <v>999000000007602</v>
+      </c>
+      <c r="E32" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
         <v>62</v>
       </c>
-      <c r="B32" s="3">
+      <c r="B33" s="3">
         <v>44472.19568287037</v>
       </c>
-      <c r="C32" s="3">
+      <c r="C33" s="3">
         <v>44475.510555555556</v>
       </c>
-      <c r="D32" s="2">
+      <c r="D33" s="2">
         <v>999000000007585</v>
       </c>
-      <c r="E32" t="s">
-        <v>109</v>
+      <c r="E33" t="s">
+        <v>120</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
colors more standardized within ptfiltered mod
</commit_message>
<xml_diff>
--- a/data/WGFP Metadata.xlsx
+++ b/data/WGFP Metadata.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="AntennaMetadata" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="126">
   <si>
     <t>Variable</t>
   </si>
@@ -394,6 +394,18 @@
   </si>
   <si>
     <t>sporadic, missed about half of marker detections during this period</t>
+  </si>
+  <si>
+    <t>Connectivity Downstream</t>
+  </si>
+  <si>
+    <t>Connectivity Side Channel</t>
+  </si>
+  <si>
+    <t>Connectivity Upstream</t>
+  </si>
+  <si>
+    <t>PressureTransducerSiteName needs to line up with the sites that are in the Pressuretransducer data</t>
   </si>
 </sst>
 </file>
@@ -717,7 +729,7 @@
   <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1082,6 +1094,9 @@
       <c r="D13" t="s">
         <v>20</v>
       </c>
+      <c r="E13" t="s">
+        <v>122</v>
+      </c>
       <c r="F13">
         <v>415802</v>
       </c>
@@ -1108,6 +1123,9 @@
       <c r="D14" t="s">
         <v>21</v>
       </c>
+      <c r="E14" t="s">
+        <v>122</v>
+      </c>
       <c r="F14">
         <v>415802</v>
       </c>
@@ -1134,6 +1152,9 @@
       <c r="D15" t="s">
         <v>22</v>
       </c>
+      <c r="E15" t="s">
+        <v>123</v>
+      </c>
       <c r="F15">
         <v>415787</v>
       </c>
@@ -1160,6 +1181,9 @@
       <c r="D16" t="s">
         <v>23</v>
       </c>
+      <c r="E16" t="s">
+        <v>123</v>
+      </c>
       <c r="F16">
         <v>415787</v>
       </c>
@@ -1186,6 +1210,9 @@
       <c r="D17" t="s">
         <v>24</v>
       </c>
+      <c r="E17" t="s">
+        <v>124</v>
+      </c>
       <c r="F17">
         <v>416723</v>
       </c>
@@ -1211,6 +1238,9 @@
       </c>
       <c r="D18" t="s">
         <v>25</v>
+      </c>
+      <c r="E18" t="s">
+        <v>124</v>
       </c>
       <c r="F18">
         <v>416723</v>
@@ -1257,7 +1287,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
@@ -1982,10 +2012,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:A6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2015,6 +2045,11 @@
         <v>75</v>
       </c>
     </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>125</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
marker tag issues in app
</commit_message>
<xml_diff>
--- a/data/WGFP Metadata.xlsx
+++ b/data/WGFP Metadata.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="AntennaMetadata" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="125">
   <si>
     <t>Variable</t>
   </si>
@@ -379,9 +379,6 @@
   </si>
   <si>
     <t>2021-08-31 17:43:55 to 2021-11-04 13:15:23, and 2022-04-06 14:09:41 to 2022-06-15 11:49:09, and 2022-08-2022 15:54:17 to 2022-11-02 12:18:19</t>
-  </si>
-  <si>
-    <t>Will be resolved with Next site visit hopefully</t>
   </si>
   <si>
     <t>believe it ran out of batteries and we couldn't get to it. Had some detections in october for some reason?</t>
@@ -1095,7 +1092,7 @@
         <v>20</v>
       </c>
       <c r="E13" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F13">
         <v>415802</v>
@@ -1124,7 +1121,7 @@
         <v>21</v>
       </c>
       <c r="E14" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F14">
         <v>415802</v>
@@ -1153,7 +1150,7 @@
         <v>22</v>
       </c>
       <c r="E15" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F15">
         <v>415787</v>
@@ -1182,7 +1179,7 @@
         <v>23</v>
       </c>
       <c r="E16" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F16">
         <v>415787</v>
@@ -1211,7 +1208,7 @@
         <v>24</v>
       </c>
       <c r="E17" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F17">
         <v>416723</v>
@@ -1240,7 +1237,7 @@
         <v>25</v>
       </c>
       <c r="E18" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F18">
         <v>416723</v>
@@ -1287,8 +1284,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1339,14 +1336,11 @@
       <c r="B3" s="3">
         <v>45059.11041666667</v>
       </c>
-      <c r="C3" t="s">
-        <v>117</v>
-      </c>
       <c r="D3" s="2">
         <v>5394</v>
       </c>
       <c r="E3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -1394,7 +1388,7 @@
         <v>5154</v>
       </c>
       <c r="E6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -1484,7 +1478,7 @@
         <v>5665</v>
       </c>
       <c r="E12" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
@@ -1754,9 +1748,6 @@
       <c r="B29" s="3">
         <v>45285.351435185185</v>
       </c>
-      <c r="C29" t="s">
-        <v>117</v>
-      </c>
       <c r="D29" s="2">
         <v>12437</v>
       </c>
@@ -1778,7 +1769,7 @@
         <v>999000000007586</v>
       </c>
       <c r="E30" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
@@ -1826,7 +1817,7 @@
         <v>999000000007585</v>
       </c>
       <c r="E33" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
   </sheetData>
@@ -2014,7 +2005,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
@@ -2047,7 +2038,7 @@
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
   </sheetData>

</xml_diff>